<commit_message>
finishing over limit file to determine if average draw is over 5 ppb
</commit_message>
<xml_diff>
--- a/wq_study_results.xlsx
+++ b/wq_study_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,8 +16,10 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Sequential!$2:$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Initial!$3:$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Initial!$3:$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Initial!$3:$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Sequential!$2:$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">Sequential!$2:$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Sequential!$2:$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2076,12 +2078,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -2199,7 +2207,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="124">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2460,31 +2468,71 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2584,6 +2632,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2608,6 +2660,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2616,8 +2672,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2948,29 +3028,29 @@
   </sheetPr>
   <dimension ref="A1:Q851"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="111.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14580,7 +14660,7 @@
       <c r="J443" s="33"/>
       <c r="K443" s="33"/>
     </row>
-    <row r="444" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="32" t="n">
         <v>42957</v>
       </c>
@@ -14601,7 +14681,7 @@
       <c r="J444" s="33"/>
       <c r="K444" s="33"/>
     </row>
-    <row r="445" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="32" t="n">
         <v>43006</v>
       </c>
@@ -14628,7 +14708,7 @@
       <c r="J445" s="33"/>
       <c r="K445" s="33"/>
     </row>
-    <row r="446" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="32" t="n">
         <v>42865</v>
       </c>
@@ -14653,7 +14733,7 @@
       <c r="J446" s="33"/>
       <c r="K446" s="33"/>
     </row>
-    <row r="447" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="32" t="n">
         <v>42970</v>
       </c>
@@ -14678,7 +14758,7 @@
       <c r="J447" s="33"/>
       <c r="K447" s="33"/>
     </row>
-    <row r="448" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="32" t="n">
         <v>42885</v>
       </c>
@@ -14703,7 +14783,7 @@
       <c r="J448" s="33"/>
       <c r="K448" s="33"/>
     </row>
-    <row r="449" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="21" t="n">
         <v>43006</v>
       </c>
@@ -14728,7 +14808,7 @@
       <c r="J449" s="23"/>
       <c r="K449" s="23"/>
     </row>
-    <row r="450" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="21" t="n">
         <v>43038</v>
       </c>
@@ -14753,7 +14833,7 @@
       <c r="J450" s="23"/>
       <c r="K450" s="23"/>
     </row>
-    <row r="451" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="21" t="n">
         <v>43067</v>
       </c>
@@ -14780,7 +14860,7 @@
       </c>
       <c r="K451" s="23"/>
     </row>
-    <row r="452" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="21" t="n">
         <v>43088</v>
       </c>
@@ -14805,7 +14885,7 @@
       <c r="J452" s="23"/>
       <c r="K452" s="23"/>
     </row>
-    <row r="453" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="21" t="n">
         <v>43059</v>
       </c>
@@ -14832,7 +14912,7 @@
       </c>
       <c r="K453" s="23"/>
     </row>
-    <row r="454" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="32" t="n">
         <v>42859</v>
       </c>
@@ -14859,7 +14939,7 @@
       <c r="J454" s="33"/>
       <c r="K454" s="33"/>
     </row>
-    <row r="455" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="32" t="n">
         <v>42893</v>
       </c>
@@ -14880,7 +14960,7 @@
       <c r="J455" s="33"/>
       <c r="K455" s="33"/>
     </row>
-    <row r="456" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="32" t="n">
         <v>43004</v>
       </c>
@@ -14907,7 +14987,7 @@
       <c r="J456" s="33"/>
       <c r="K456" s="33"/>
     </row>
-    <row r="457" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="32" t="n">
         <v>42860</v>
       </c>
@@ -14934,7 +15014,7 @@
       <c r="J457" s="33"/>
       <c r="K457" s="33"/>
     </row>
-    <row r="458" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="21" t="n">
         <v>43000</v>
       </c>
@@ -14961,7 +15041,7 @@
       <c r="J458" s="23"/>
       <c r="K458" s="23"/>
     </row>
-    <row r="459" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="32" t="n">
         <v>42860</v>
       </c>
@@ -14988,7 +15068,7 @@
       <c r="J459" s="33"/>
       <c r="K459" s="33"/>
     </row>
-    <row r="460" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="32" t="n">
         <v>42676</v>
       </c>
@@ -15013,7 +15093,7 @@
       <c r="J460" s="33"/>
       <c r="K460" s="33"/>
     </row>
-    <row r="461" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="32" t="n">
         <v>42811</v>
       </c>
@@ -15038,7 +15118,7 @@
       <c r="J461" s="33"/>
       <c r="K461" s="33"/>
     </row>
-    <row r="462" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="32" t="n">
         <v>42923</v>
       </c>
@@ -15065,7 +15145,7 @@
       <c r="J462" s="33"/>
       <c r="K462" s="33"/>
     </row>
-    <row r="463" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="21" t="n">
         <v>43007</v>
       </c>
@@ -15092,7 +15172,7 @@
       <c r="J463" s="23"/>
       <c r="K463" s="23"/>
     </row>
-    <row r="464" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="21" t="n">
         <v>43028</v>
       </c>
@@ -15119,7 +15199,7 @@
       <c r="J464" s="23"/>
       <c r="K464" s="23"/>
     </row>
-    <row r="465" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="21" t="n">
         <v>43067</v>
       </c>
@@ -15146,7 +15226,7 @@
       <c r="J465" s="23"/>
       <c r="K465" s="23"/>
     </row>
-    <row r="466" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="21" t="n">
         <v>43084</v>
       </c>
@@ -15173,7 +15253,7 @@
       <c r="J466" s="23"/>
       <c r="K466" s="23"/>
     </row>
-    <row r="467" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="32" t="n">
         <v>42922</v>
       </c>
@@ -15200,7 +15280,7 @@
       <c r="J467" s="33"/>
       <c r="K467" s="33"/>
     </row>
-    <row r="468" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="21" t="n">
         <v>43007</v>
       </c>
@@ -15229,7 +15309,7 @@
       </c>
       <c r="K468" s="23"/>
     </row>
-    <row r="469" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="21" t="n">
         <v>43028</v>
       </c>
@@ -15258,7 +15338,7 @@
       </c>
       <c r="K469" s="23"/>
     </row>
-    <row r="470" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="21" t="n">
         <v>43056</v>
       </c>
@@ -25199,137 +25279,137 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>S9="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>S10="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>S7="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>S8="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:E14">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>R14="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:E16">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>R16="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:E17">
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>R17="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C530:E530">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>M532="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B400:E400">
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>L394="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B401:E401">
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>L395="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B389:E389">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>S385="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:E18">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>R18="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>S11="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B532:E532">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>L534="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B531:E531">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>L533="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B545:E545">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>I545="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B390:E390">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>S386="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B391:E391">
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>S387="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B396:E396">
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
       <formula>L391="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B543:E543">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>I543="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B385:E386">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
       <formula>S381="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>R7="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>R10="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:D8">
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>R8="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:D11">
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>R11="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B404">
-    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
       <formula>L398="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B405">
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
       <formula>L399="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25354,25 +25434,24 @@
   </sheetPr>
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="true" max="5" min="4" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1122448979592"/>
+    <col collapsed="false" hidden="true" max="7" min="7" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="true" max="13" min="9" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="true" max="17" min="15" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -25471,149 +25550,149 @@
         <v>545</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="n">
+    <row r="4" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="65" t="n">
         <v>42651</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="66" t="s">
         <v>546</v>
       </c>
-      <c r="C4" s="65" t="n">
+      <c r="C4" s="67" t="n">
         <v>2.19</v>
       </c>
-      <c r="D4" s="65" t="n">
+      <c r="D4" s="67" t="n">
         <v>2.26</v>
       </c>
-      <c r="E4" s="65" t="n">
+      <c r="E4" s="67" t="n">
         <v>4.07</v>
       </c>
-      <c r="F4" s="66" t="n">
+      <c r="F4" s="68" t="n">
         <v>3.71</v>
       </c>
-      <c r="G4" s="65" t="n">
+      <c r="G4" s="67" t="n">
         <v>9.38</v>
       </c>
-      <c r="H4" s="65" t="n">
+      <c r="H4" s="67" t="n">
         <v>15.4</v>
       </c>
-      <c r="I4" s="65" t="n">
+      <c r="I4" s="67" t="n">
         <v>11.5</v>
       </c>
-      <c r="J4" s="65" t="n">
+      <c r="J4" s="67" t="n">
         <v>10.5</v>
       </c>
-      <c r="K4" s="65" t="n">
+      <c r="K4" s="67" t="n">
         <v>11.2</v>
       </c>
-      <c r="L4" s="65" t="n">
+      <c r="L4" s="67" t="n">
         <v>10.2</v>
       </c>
-      <c r="M4" s="65" t="n">
+      <c r="M4" s="67" t="n">
         <v>8.35</v>
       </c>
-      <c r="N4" s="67" t="n">
+      <c r="N4" s="69" t="n">
         <v>4.36</v>
       </c>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="29"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="n">
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="70"/>
+    </row>
+    <row r="5" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="72" t="n">
         <v>42984</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="73" t="s">
         <v>547</v>
       </c>
-      <c r="C5" s="68" t="n">
+      <c r="C5" s="74" t="n">
         <v>57.1</v>
       </c>
-      <c r="D5" s="31" t="n">
+      <c r="D5" s="75" t="n">
         <v>28.7</v>
       </c>
-      <c r="E5" s="31" t="n">
+      <c r="E5" s="75" t="n">
         <v>25.1</v>
       </c>
-      <c r="F5" s="31" t="n">
+      <c r="F5" s="75" t="n">
         <v>22.1</v>
       </c>
-      <c r="G5" s="31" t="n">
+      <c r="G5" s="75" t="n">
         <v>20.2</v>
       </c>
-      <c r="H5" s="31" t="n">
+      <c r="H5" s="75" t="n">
         <v>18.9</v>
       </c>
-      <c r="I5" s="31" t="n">
+      <c r="I5" s="75" t="n">
         <v>16.8</v>
       </c>
-      <c r="J5" s="31" t="n">
+      <c r="J5" s="75" t="n">
         <v>17.6</v>
       </c>
-      <c r="K5" s="31" t="n">
+      <c r="K5" s="75" t="n">
         <v>15.4</v>
       </c>
-      <c r="L5" s="31" t="n">
+      <c r="L5" s="75" t="n">
         <v>14.1</v>
       </c>
-      <c r="M5" s="29" t="n">
+      <c r="M5" s="70" t="n">
         <v>5.32</v>
       </c>
-      <c r="N5" s="29" t="n">
+      <c r="N5" s="70" t="n">
         <v>4.28</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="69" t="n">
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+    </row>
+    <row r="6" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="76" t="n">
         <v>43050</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="73" t="s">
         <v>548</v>
       </c>
-      <c r="C6" s="70" t="n">
+      <c r="C6" s="77" t="n">
         <v>8.99</v>
       </c>
-      <c r="D6" s="70" t="n">
+      <c r="D6" s="77" t="n">
         <v>5.63</v>
       </c>
-      <c r="E6" s="70" t="n">
+      <c r="E6" s="77" t="n">
         <v>6.87</v>
       </c>
-      <c r="F6" s="70" t="n">
+      <c r="F6" s="77" t="n">
         <v>23.9</v>
       </c>
-      <c r="G6" s="70" t="n">
+      <c r="G6" s="77" t="n">
         <v>18.1</v>
       </c>
-      <c r="H6" s="71" t="n">
+      <c r="H6" s="78" t="n">
         <v>12.1</v>
       </c>
-      <c r="I6" s="42" t="n">
+      <c r="I6" s="79" t="n">
         <v>17.3</v>
       </c>
-      <c r="J6" s="46" t="n">
+      <c r="J6" s="80" t="n">
         <v>11</v>
       </c>
-      <c r="K6" s="70" t="n">
+      <c r="K6" s="77" t="n">
         <v>8.41</v>
       </c>
-      <c r="L6" s="70" t="n">
+      <c r="L6" s="77" t="n">
         <v>6.96</v>
       </c>
-      <c r="M6" s="70" t="n">
+      <c r="M6" s="77" t="n">
         <v>6.39</v>
       </c>
-      <c r="N6" s="70" t="n">
+      <c r="N6" s="77" t="n">
         <v>5.23</v>
       </c>
-      <c r="O6" s="70"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="42"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="79"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="69" t="n">
+      <c r="A7" s="81" t="n">
         <v>43056</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -25634,7 +25713,7 @@
       <c r="G7" s="39" t="n">
         <v>19.3</v>
       </c>
-      <c r="H7" s="72" t="n">
+      <c r="H7" s="82" t="n">
         <v>20.8</v>
       </c>
       <c r="I7" s="22" t="n">
@@ -25655,51 +25734,51 @@
       <c r="N7" s="39" t="n">
         <v>8.7</v>
       </c>
-      <c r="O7" s="73"/>
-      <c r="P7" s="72"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="82"/>
       <c r="Q7" s="22"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="69" t="n">
+      <c r="A8" s="81" t="n">
         <v>43105</v>
       </c>
       <c r="B8" s="46" t="s">
         <v>550</v>
       </c>
-      <c r="C8" s="74" t="n">
+      <c r="C8" s="84" t="n">
         <v>4.46</v>
       </c>
-      <c r="D8" s="75" t="n">
+      <c r="D8" s="85" t="n">
         <v>2.99</v>
       </c>
-      <c r="E8" s="75" t="n">
+      <c r="E8" s="85" t="n">
         <v>3.48</v>
       </c>
-      <c r="F8" s="75" t="n">
+      <c r="F8" s="85" t="n">
         <v>5.18</v>
       </c>
-      <c r="G8" s="76" t="n">
+      <c r="G8" s="86" t="n">
         <v>4.56</v>
       </c>
-      <c r="H8" s="76" t="n">
+      <c r="H8" s="86" t="n">
         <v>4.52</v>
       </c>
-      <c r="I8" s="76" t="n">
+      <c r="I8" s="86" t="n">
         <v>5.94</v>
       </c>
-      <c r="J8" s="75" t="n">
+      <c r="J8" s="85" t="n">
         <v>6.8</v>
       </c>
-      <c r="K8" s="76" t="n">
+      <c r="K8" s="86" t="n">
         <v>6.71</v>
       </c>
-      <c r="L8" s="76" t="n">
+      <c r="L8" s="86" t="n">
         <v>6.69</v>
       </c>
-      <c r="M8" s="76" t="n">
+      <c r="M8" s="86" t="n">
         <v>2.65</v>
       </c>
-      <c r="N8" s="76" t="n">
+      <c r="N8" s="86" t="n">
         <v>1.74</v>
       </c>
       <c r="O8" s="51"/>
@@ -25713,66 +25792,66 @@
       <c r="B9" s="25" t="s">
         <v>551</v>
       </c>
-      <c r="C9" s="77" t="n">
+      <c r="C9" s="87" t="n">
         <v>23</v>
       </c>
-      <c r="D9" s="78" t="n">
+      <c r="D9" s="88" t="n">
         <v>5.23</v>
       </c>
-      <c r="E9" s="78" t="n">
+      <c r="E9" s="88" t="n">
         <v>4.29</v>
       </c>
-      <c r="F9" s="78" t="n">
+      <c r="F9" s="88" t="n">
         <v>4.56</v>
       </c>
-      <c r="G9" s="78" t="n">
+      <c r="G9" s="88" t="n">
         <v>4.53</v>
       </c>
-      <c r="H9" s="78" t="n">
+      <c r="H9" s="88" t="n">
         <v>3.48</v>
       </c>
-      <c r="I9" s="78" t="n">
+      <c r="I9" s="88" t="n">
         <v>9.66</v>
       </c>
-      <c r="J9" s="78" t="n">
+      <c r="J9" s="88" t="n">
         <v>8.68</v>
       </c>
-      <c r="K9" s="78" t="n">
+      <c r="K9" s="88" t="n">
         <v>8.57</v>
       </c>
-      <c r="L9" s="78" t="n">
+      <c r="L9" s="88" t="n">
         <v>6.81</v>
       </c>
-      <c r="M9" s="78" t="n">
+      <c r="M9" s="88" t="n">
         <v>3.92</v>
       </c>
-      <c r="N9" s="78" t="n">
+      <c r="N9" s="88" t="n">
         <v>3.32</v>
       </c>
       <c r="O9" s="51"/>
       <c r="P9" s="51"/>
-      <c r="Q9" s="79"/>
+      <c r="Q9" s="89"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="28" t="n">
         <v>42676</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="90" t="s">
         <v>552</v>
       </c>
-      <c r="C10" s="81" t="n">
+      <c r="C10" s="91" t="n">
         <v>5.07</v>
       </c>
-      <c r="D10" s="81" t="n">
+      <c r="D10" s="91" t="n">
         <v>5.72</v>
       </c>
-      <c r="E10" s="81" t="n">
+      <c r="E10" s="91" t="n">
         <v>3.06</v>
       </c>
-      <c r="F10" s="81" t="n">
+      <c r="F10" s="91" t="n">
         <v>2.65</v>
       </c>
-      <c r="G10" s="81" t="n">
+      <c r="G10" s="91" t="n">
         <v>6.3</v>
       </c>
       <c r="H10" s="20" t="n">
@@ -25787,13 +25866,13 @@
       <c r="K10" s="20" t="n">
         <v>12.4</v>
       </c>
-      <c r="L10" s="81" t="n">
+      <c r="L10" s="91" t="n">
         <v>5.7</v>
       </c>
-      <c r="M10" s="81" t="n">
+      <c r="M10" s="91" t="n">
         <v>4.22</v>
       </c>
-      <c r="N10" s="81" t="n">
+      <c r="N10" s="91" t="n">
         <v>3.15</v>
       </c>
       <c r="O10" s="14"/>
@@ -25801,108 +25880,108 @@
       <c r="Q10" s="29"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="82" t="n">
+      <c r="A11" s="92" t="n">
         <v>42951</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="86" t="s">
         <v>553</v>
       </c>
-      <c r="C11" s="74" t="n">
+      <c r="C11" s="84" t="n">
         <v>1.61</v>
       </c>
-      <c r="D11" s="83" t="n">
+      <c r="D11" s="93" t="n">
         <v>2.1</v>
       </c>
-      <c r="E11" s="83" t="n">
+      <c r="E11" s="93" t="n">
         <v>1.65</v>
       </c>
-      <c r="F11" s="84" t="s">
+      <c r="F11" s="94" t="s">
         <v>554</v>
       </c>
-      <c r="G11" s="85" t="s">
+      <c r="G11" s="95" t="s">
         <v>554</v>
       </c>
-      <c r="H11" s="85" t="s">
+      <c r="H11" s="95" t="s">
         <v>554</v>
       </c>
-      <c r="I11" s="85" t="s">
+      <c r="I11" s="95" t="s">
         <v>554</v>
       </c>
-      <c r="J11" s="85" t="s">
+      <c r="J11" s="95" t="s">
         <v>554</v>
       </c>
-      <c r="K11" s="85" t="s">
+      <c r="K11" s="95" t="s">
         <v>554</v>
       </c>
-      <c r="L11" s="85" t="s">
+      <c r="L11" s="95" t="s">
         <v>554</v>
       </c>
-      <c r="M11" s="85" t="s">
+      <c r="M11" s="95" t="s">
         <v>554</v>
       </c>
-      <c r="N11" s="85" t="s">
+      <c r="N11" s="95" t="s">
         <v>554</v>
       </c>
-      <c r="O11" s="86" t="s">
+      <c r="O11" s="96" t="s">
         <v>554</v>
       </c>
-      <c r="P11" s="86" t="s">
+      <c r="P11" s="96" t="s">
         <v>554</v>
       </c>
-      <c r="Q11" s="86" t="s">
+      <c r="Q11" s="96" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="87" t="n">
+      <c r="A12" s="97" t="n">
         <v>42832</v>
       </c>
       <c r="B12" s="46" t="s">
         <v>555</v>
       </c>
-      <c r="C12" s="77" t="n">
+      <c r="C12" s="87" t="n">
         <v>10.4</v>
       </c>
-      <c r="D12" s="77" t="n">
+      <c r="D12" s="87" t="n">
         <v>15.6</v>
       </c>
-      <c r="E12" s="77" t="n">
+      <c r="E12" s="87" t="n">
         <v>14.2</v>
       </c>
-      <c r="F12" s="77" t="n">
+      <c r="F12" s="87" t="n">
         <v>11.9</v>
       </c>
-      <c r="G12" s="78" t="n">
+      <c r="G12" s="88" t="n">
         <v>11.1</v>
       </c>
-      <c r="H12" s="78" t="n">
+      <c r="H12" s="88" t="n">
         <v>10.2</v>
       </c>
-      <c r="I12" s="78" t="n">
+      <c r="I12" s="88" t="n">
         <v>9.54</v>
       </c>
-      <c r="J12" s="78" t="n">
+      <c r="J12" s="88" t="n">
         <v>8.5</v>
       </c>
-      <c r="K12" s="78" t="n">
+      <c r="K12" s="88" t="n">
         <v>8.41</v>
       </c>
-      <c r="L12" s="78" t="n">
+      <c r="L12" s="88" t="n">
         <v>6.53</v>
       </c>
-      <c r="M12" s="78" t="n">
+      <c r="M12" s="88" t="n">
         <v>5.33</v>
       </c>
-      <c r="N12" s="78" t="n">
+      <c r="N12" s="88" t="n">
         <v>4.94</v>
       </c>
-      <c r="O12" s="88" t="n">
+      <c r="O12" s="98" t="n">
         <v>4.6</v>
       </c>
       <c r="P12" s="51" t="n">
         <v>4.49</v>
       </c>
-      <c r="Q12" s="79" t="n">
+      <c r="Q12" s="89" t="n">
         <v>4.32</v>
       </c>
     </row>
@@ -25910,66 +25989,66 @@
       <c r="A13" s="28" t="n">
         <v>42797</v>
       </c>
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="99" t="s">
         <v>556</v>
       </c>
-      <c r="C13" s="78" t="n">
+      <c r="C13" s="88" t="n">
         <v>4.07</v>
       </c>
-      <c r="D13" s="78" t="n">
+      <c r="D13" s="88" t="n">
         <v>3.18</v>
       </c>
-      <c r="E13" s="78" t="n">
+      <c r="E13" s="88" t="n">
         <v>3.16</v>
       </c>
-      <c r="F13" s="78" t="n">
+      <c r="F13" s="88" t="n">
         <v>2.4</v>
       </c>
-      <c r="G13" s="78" t="n">
+      <c r="G13" s="88" t="n">
         <v>3.44</v>
       </c>
-      <c r="H13" s="78" t="n">
+      <c r="H13" s="88" t="n">
         <v>3.92</v>
       </c>
-      <c r="I13" s="78" t="n">
+      <c r="I13" s="88" t="n">
         <v>2.6</v>
       </c>
-      <c r="J13" s="78" t="n">
+      <c r="J13" s="88" t="n">
         <v>4.04</v>
       </c>
-      <c r="K13" s="78" t="n">
+      <c r="K13" s="88" t="n">
         <v>2.73</v>
       </c>
-      <c r="L13" s="78" t="n">
+      <c r="L13" s="88" t="n">
         <v>5.05</v>
       </c>
-      <c r="M13" s="78" t="n">
+      <c r="M13" s="88" t="n">
         <v>3.05</v>
       </c>
-      <c r="N13" s="78" t="n">
+      <c r="N13" s="88" t="n">
         <v>1.36</v>
       </c>
       <c r="O13" s="51"/>
       <c r="P13" s="51"/>
-      <c r="Q13" s="79"/>
+      <c r="Q13" s="89"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="82" t="n">
+      <c r="A14" s="92" t="n">
         <v>42949</v>
       </c>
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="100" t="s">
         <v>557</v>
       </c>
-      <c r="C14" s="81" t="n">
+      <c r="C14" s="91" t="n">
         <v>9.55</v>
       </c>
-      <c r="D14" s="81" t="n">
+      <c r="D14" s="91" t="n">
         <v>9.54</v>
       </c>
-      <c r="E14" s="81" t="n">
+      <c r="E14" s="91" t="n">
         <v>9.15</v>
       </c>
-      <c r="F14" s="81" t="n">
+      <c r="F14" s="91" t="n">
         <v>9.45</v>
       </c>
       <c r="G14" s="20" t="n">
@@ -25993,7 +26072,7 @@
       <c r="M14" s="20" t="n">
         <v>23.2</v>
       </c>
-      <c r="N14" s="81" t="n">
+      <c r="N14" s="91" t="n">
         <v>8.76</v>
       </c>
       <c r="O14" s="29" t="n">
@@ -26007,55 +26086,55 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="82" t="n">
+      <c r="A15" s="92" t="n">
         <v>42997</v>
       </c>
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="100" t="s">
         <v>558</v>
       </c>
-      <c r="C15" s="91" t="n">
+      <c r="C15" s="101" t="n">
         <v>6.31</v>
       </c>
-      <c r="D15" s="92" t="n">
+      <c r="D15" s="102" t="n">
         <v>8.05</v>
       </c>
-      <c r="E15" s="92" t="n">
+      <c r="E15" s="102" t="n">
         <v>7.46</v>
       </c>
-      <c r="F15" s="92" t="n">
+      <c r="F15" s="102" t="n">
         <v>8.4</v>
       </c>
-      <c r="G15" s="93" t="n">
+      <c r="G15" s="103" t="n">
         <v>11.2</v>
       </c>
-      <c r="H15" s="93" t="n">
+      <c r="H15" s="103" t="n">
         <v>14.1</v>
       </c>
-      <c r="I15" s="93" t="n">
+      <c r="I15" s="103" t="n">
         <v>15.7</v>
       </c>
-      <c r="J15" s="93" t="n">
+      <c r="J15" s="103" t="n">
         <v>15.6</v>
       </c>
-      <c r="K15" s="93" t="s">
+      <c r="K15" s="103" t="s">
         <v>559</v>
       </c>
-      <c r="L15" s="86" t="s">
+      <c r="L15" s="96" t="s">
         <v>559</v>
       </c>
-      <c r="M15" s="93" t="n">
+      <c r="M15" s="103" t="n">
         <v>15.2</v>
       </c>
-      <c r="N15" s="86" t="n">
+      <c r="N15" s="96" t="n">
         <v>27</v>
       </c>
-      <c r="O15" s="94" t="n">
+      <c r="O15" s="104" t="n">
         <v>4.99</v>
       </c>
-      <c r="P15" s="93" t="n">
+      <c r="P15" s="103" t="n">
         <v>4.15</v>
       </c>
-      <c r="Q15" s="92" t="n">
+      <c r="Q15" s="102" t="n">
         <v>4.01</v>
       </c>
     </row>
@@ -26066,49 +26145,49 @@
       <c r="B16" s="14" t="s">
         <v>560</v>
       </c>
-      <c r="C16" s="95" t="n">
+      <c r="C16" s="105" t="n">
         <v>24</v>
       </c>
-      <c r="D16" s="95" t="n">
+      <c r="D16" s="105" t="n">
         <v>28.8</v>
       </c>
-      <c r="E16" s="95" t="n">
+      <c r="E16" s="105" t="n">
         <v>58.2</v>
       </c>
-      <c r="F16" s="95" t="n">
+      <c r="F16" s="105" t="n">
         <v>29</v>
       </c>
-      <c r="G16" s="95" t="n">
+      <c r="G16" s="105" t="n">
         <v>21.7</v>
       </c>
-      <c r="H16" s="95" t="n">
+      <c r="H16" s="105" t="n">
         <v>20.3</v>
       </c>
-      <c r="I16" s="95" t="n">
+      <c r="I16" s="105" t="n">
         <v>20.1</v>
       </c>
-      <c r="J16" s="95" t="n">
+      <c r="J16" s="105" t="n">
         <v>13.1</v>
       </c>
-      <c r="K16" s="95" t="n">
+      <c r="K16" s="105" t="n">
         <v>10.5</v>
       </c>
-      <c r="L16" s="95" t="n">
+      <c r="L16" s="105" t="n">
         <v>9.82</v>
       </c>
-      <c r="M16" s="95" t="n">
+      <c r="M16" s="105" t="n">
         <v>9.51</v>
       </c>
-      <c r="N16" s="95" t="n">
+      <c r="N16" s="105" t="n">
         <v>8.93</v>
       </c>
-      <c r="O16" s="65" t="n">
+      <c r="O16" s="106" t="n">
         <v>8.77</v>
       </c>
-      <c r="P16" s="65" t="n">
+      <c r="P16" s="106" t="n">
         <v>8.33</v>
       </c>
-      <c r="Q16" s="65" t="n">
+      <c r="Q16" s="106" t="n">
         <v>7.95</v>
       </c>
     </row>
@@ -26119,87 +26198,87 @@
       <c r="B17" s="25" t="s">
         <v>561</v>
       </c>
-      <c r="C17" s="96" t="n">
+      <c r="C17" s="107" t="n">
         <v>6.19</v>
       </c>
-      <c r="D17" s="96" t="n">
+      <c r="D17" s="107" t="n">
         <v>2.55</v>
       </c>
-      <c r="E17" s="96" t="n">
+      <c r="E17" s="107" t="n">
         <v>4.78</v>
       </c>
-      <c r="F17" s="96" t="n">
+      <c r="F17" s="107" t="n">
         <v>2.27</v>
       </c>
-      <c r="G17" s="97" t="n">
+      <c r="G17" s="108" t="n">
         <v>2.3</v>
       </c>
-      <c r="H17" s="96" t="n">
+      <c r="H17" s="107" t="n">
         <v>2.58</v>
       </c>
-      <c r="I17" s="96" t="n">
+      <c r="I17" s="107" t="n">
         <v>4.33</v>
       </c>
-      <c r="J17" s="96" t="n">
+      <c r="J17" s="107" t="n">
         <v>2.22</v>
       </c>
-      <c r="K17" s="96" t="n">
+      <c r="K17" s="107" t="n">
         <v>2.13</v>
       </c>
-      <c r="L17" s="96" t="n">
+      <c r="L17" s="107" t="n">
         <v>2.13</v>
       </c>
-      <c r="M17" s="96" t="n">
+      <c r="M17" s="107" t="n">
         <v>1.96</v>
       </c>
-      <c r="N17" s="96" t="n">
+      <c r="N17" s="107" t="n">
         <v>1.91</v>
       </c>
       <c r="O17" s="51"/>
       <c r="P17" s="51"/>
-      <c r="Q17" s="79"/>
+      <c r="Q17" s="89"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="n">
         <v>42882</v>
       </c>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="109" t="s">
         <v>562</v>
       </c>
-      <c r="C18" s="96" t="n">
+      <c r="C18" s="107" t="n">
         <v>5.2</v>
       </c>
-      <c r="D18" s="96" t="n">
+      <c r="D18" s="107" t="n">
         <v>6.06</v>
       </c>
-      <c r="E18" s="96" t="n">
+      <c r="E18" s="107" t="n">
         <v>5.11</v>
       </c>
-      <c r="F18" s="96" t="n">
+      <c r="F18" s="107" t="n">
         <v>7.11</v>
       </c>
-      <c r="G18" s="96" t="n">
+      <c r="G18" s="107" t="n">
         <v>6.05</v>
       </c>
-      <c r="H18" s="96" t="n">
+      <c r="H18" s="107" t="n">
         <v>4.51</v>
       </c>
-      <c r="I18" s="96" t="n">
+      <c r="I18" s="107" t="n">
         <v>4.96</v>
       </c>
-      <c r="J18" s="96" t="n">
+      <c r="J18" s="107" t="n">
         <v>3.55</v>
       </c>
-      <c r="K18" s="96" t="n">
+      <c r="K18" s="107" t="n">
         <v>3.49</v>
       </c>
-      <c r="L18" s="96" t="n">
+      <c r="L18" s="107" t="n">
         <v>2.22</v>
       </c>
-      <c r="M18" s="97" t="n">
+      <c r="M18" s="108" t="n">
         <v>2</v>
       </c>
-      <c r="N18" s="96" t="n">
+      <c r="N18" s="107" t="n">
         <v>1.57</v>
       </c>
       <c r="O18" s="14"/>
@@ -26207,102 +26286,102 @@
       <c r="Q18" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="99" t="n">
+      <c r="A19" s="110" t="n">
         <v>42882</v>
       </c>
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="111" t="s">
         <v>563</v>
       </c>
-      <c r="C19" s="96" t="n">
+      <c r="C19" s="107" t="n">
         <v>13.9</v>
       </c>
-      <c r="D19" s="96" t="n">
+      <c r="D19" s="107" t="n">
         <v>23.1</v>
       </c>
-      <c r="E19" s="96" t="n">
+      <c r="E19" s="107" t="n">
         <v>39.8</v>
       </c>
-      <c r="F19" s="96" t="n">
+      <c r="F19" s="107" t="n">
         <v>26.7</v>
       </c>
-      <c r="G19" s="96" t="n">
+      <c r="G19" s="107" t="n">
         <v>27</v>
       </c>
-      <c r="H19" s="96" t="n">
+      <c r="H19" s="107" t="n">
         <v>25.3</v>
       </c>
-      <c r="I19" s="96" t="n">
+      <c r="I19" s="107" t="n">
         <v>24.9</v>
       </c>
-      <c r="J19" s="96" t="n">
+      <c r="J19" s="107" t="n">
         <v>24.7</v>
       </c>
-      <c r="K19" s="96" t="n">
+      <c r="K19" s="107" t="n">
         <v>33.1</v>
       </c>
-      <c r="L19" s="96" t="n">
+      <c r="L19" s="107" t="n">
         <v>17.4</v>
       </c>
-      <c r="M19" s="96" t="n">
+      <c r="M19" s="107" t="n">
         <v>6.18</v>
       </c>
-      <c r="N19" s="96" t="n">
+      <c r="N19" s="107" t="n">
         <v>5.3</v>
       </c>
-      <c r="O19" s="94"/>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="92"/>
+      <c r="O19" s="104"/>
+      <c r="P19" s="103"/>
+      <c r="Q19" s="102"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="n">
         <v>42957</v>
       </c>
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="109" t="s">
         <v>563</v>
       </c>
-      <c r="C20" s="65" t="n">
+      <c r="C20" s="106" t="n">
         <v>14.3</v>
       </c>
-      <c r="D20" s="65" t="n">
+      <c r="D20" s="106" t="n">
         <v>21.7</v>
       </c>
-      <c r="E20" s="65" t="n">
+      <c r="E20" s="106" t="n">
         <v>28.2</v>
       </c>
-      <c r="F20" s="65" t="n">
+      <c r="F20" s="106" t="n">
         <v>29.6</v>
       </c>
-      <c r="G20" s="65" t="n">
+      <c r="G20" s="106" t="n">
         <v>30.5</v>
       </c>
-      <c r="H20" s="65" t="n">
+      <c r="H20" s="106" t="n">
         <v>30</v>
       </c>
-      <c r="I20" s="65" t="n">
+      <c r="I20" s="106" t="n">
         <v>33.6</v>
       </c>
-      <c r="J20" s="65" t="n">
+      <c r="J20" s="106" t="n">
         <v>38.6</v>
       </c>
-      <c r="K20" s="65" t="n">
+      <c r="K20" s="106" t="n">
         <v>34.8</v>
       </c>
-      <c r="L20" s="65" t="n">
+      <c r="L20" s="106" t="n">
         <v>32.1</v>
       </c>
-      <c r="M20" s="65" t="n">
+      <c r="M20" s="106" t="n">
         <v>10.4</v>
       </c>
-      <c r="N20" s="65" t="n">
+      <c r="N20" s="106" t="n">
         <v>8.32</v>
       </c>
-      <c r="O20" s="101" t="n">
+      <c r="O20" s="112" t="n">
         <v>8.04</v>
       </c>
-      <c r="P20" s="96" t="n">
+      <c r="P20" s="107" t="n">
         <v>7.87</v>
       </c>
-      <c r="Q20" s="96" t="n">
+      <c r="Q20" s="107" t="n">
         <v>7.61</v>
       </c>
     </row>
@@ -26313,40 +26392,40 @@
       <c r="B21" s="14" t="s">
         <v>564</v>
       </c>
-      <c r="C21" s="65" t="n">
+      <c r="C21" s="106" t="n">
         <v>177</v>
       </c>
-      <c r="D21" s="65" t="n">
+      <c r="D21" s="106" t="n">
         <v>93.4</v>
       </c>
-      <c r="E21" s="65" t="n">
+      <c r="E21" s="106" t="n">
         <v>123</v>
       </c>
-      <c r="F21" s="65" t="n">
+      <c r="F21" s="106" t="n">
         <v>110</v>
       </c>
-      <c r="G21" s="65" t="n">
+      <c r="G21" s="106" t="n">
         <v>84.1</v>
       </c>
-      <c r="H21" s="65" t="n">
+      <c r="H21" s="106" t="n">
         <v>70.9</v>
       </c>
-      <c r="I21" s="65" t="n">
+      <c r="I21" s="106" t="n">
         <v>41.5</v>
       </c>
-      <c r="J21" s="65" t="n">
+      <c r="J21" s="106" t="n">
         <v>22.7</v>
       </c>
-      <c r="K21" s="65" t="n">
+      <c r="K21" s="106" t="n">
         <v>42.5</v>
       </c>
-      <c r="L21" s="65" t="n">
+      <c r="L21" s="106" t="n">
         <v>52.9</v>
       </c>
-      <c r="M21" s="65" t="n">
+      <c r="M21" s="106" t="n">
         <v>9.93</v>
       </c>
-      <c r="N21" s="65" t="n">
+      <c r="N21" s="106" t="n">
         <v>7.82</v>
       </c>
       <c r="O21" s="14"/>
@@ -26354,13 +26433,13 @@
       <c r="Q21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="69" t="n">
+      <c r="A22" s="81" t="n">
         <v>43061</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>565</v>
       </c>
-      <c r="C22" s="68" t="n">
+      <c r="C22" s="113" t="n">
         <v>12.7</v>
       </c>
       <c r="D22" s="31" t="n">
@@ -26401,7 +26480,7 @@
       <c r="Q22" s="29"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="102" t="n">
+      <c r="A23" s="114" t="n">
         <v>43047</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -26422,7 +26501,7 @@
       <c r="G23" s="39" t="n">
         <v>15</v>
       </c>
-      <c r="H23" s="72" t="n">
+      <c r="H23" s="82" t="n">
         <v>13.3</v>
       </c>
       <c r="I23" s="22" t="n">
@@ -26444,14 +26523,14 @@
         <v>3.37</v>
       </c>
       <c r="O23" s="39"/>
-      <c r="P23" s="72"/>
+      <c r="P23" s="82"/>
       <c r="Q23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="99" t="n">
+      <c r="A24" s="110" t="n">
         <v>42672</v>
       </c>
-      <c r="B24" s="89" t="s">
+      <c r="B24" s="99" t="s">
         <v>567</v>
       </c>
       <c r="C24" s="20" t="n">
@@ -26484,10 +26563,10 @@
       <c r="L24" s="20" t="n">
         <v>21.4</v>
       </c>
-      <c r="M24" s="81" t="n">
+      <c r="M24" s="91" t="n">
         <v>4.78</v>
       </c>
-      <c r="N24" s="81" t="n">
+      <c r="N24" s="91" t="n">
         <v>4.35</v>
       </c>
       <c r="O24" s="14"/>
@@ -26495,7 +26574,7 @@
       <c r="Q24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="102" t="n">
+      <c r="A25" s="114" t="n">
         <v>42994</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -26516,7 +26595,7 @@
       <c r="G25" s="39" t="n">
         <v>24.3</v>
       </c>
-      <c r="H25" s="72" t="n">
+      <c r="H25" s="82" t="n">
         <v>21.2</v>
       </c>
       <c r="I25" s="22" t="n">
@@ -26540,7 +26619,7 @@
       <c r="O25" s="39" t="n">
         <v>5.59</v>
       </c>
-      <c r="P25" s="72" t="n">
+      <c r="P25" s="82" t="n">
         <v>5.59</v>
       </c>
       <c r="Q25" s="22" t="n">
@@ -26548,7 +26627,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="102" t="n">
+      <c r="A26" s="114" t="n">
         <v>43034</v>
       </c>
       <c r="B26" s="25" t="s">
@@ -26569,7 +26648,7 @@
       <c r="G26" s="39" t="n">
         <v>8.14</v>
       </c>
-      <c r="H26" s="72" t="n">
+      <c r="H26" s="82" t="n">
         <v>9.04</v>
       </c>
       <c r="I26" s="22" t="n">
@@ -26593,7 +26672,7 @@
       <c r="O26" s="39" t="n">
         <v>6.38</v>
       </c>
-      <c r="P26" s="72" t="n">
+      <c r="P26" s="82" t="n">
         <v>5.53</v>
       </c>
       <c r="Q26" s="22" t="n">
@@ -26607,7 +26686,7 @@
       <c r="B27" s="25" t="s">
         <v>570</v>
       </c>
-      <c r="C27" s="81" t="n">
+      <c r="C27" s="91" t="n">
         <v>3.95</v>
       </c>
       <c r="D27" s="20" t="n">
@@ -26628,19 +26707,19 @@
       <c r="I27" s="20" t="n">
         <v>12.6</v>
       </c>
-      <c r="J27" s="81" t="n">
+      <c r="J27" s="91" t="n">
         <v>9.49</v>
       </c>
-      <c r="K27" s="81" t="n">
+      <c r="K27" s="91" t="n">
         <v>5.98</v>
       </c>
-      <c r="L27" s="81" t="n">
+      <c r="L27" s="91" t="n">
         <v>3.22</v>
       </c>
-      <c r="M27" s="81" t="n">
+      <c r="M27" s="91" t="n">
         <v>3.06</v>
       </c>
-      <c r="N27" s="81" t="n">
+      <c r="N27" s="91" t="n">
         <v>1.99</v>
       </c>
       <c r="O27" s="14"/>
@@ -26654,40 +26733,40 @@
       <c r="B28" s="25" t="s">
         <v>570</v>
       </c>
-      <c r="C28" s="65" t="n">
+      <c r="C28" s="106" t="n">
         <v>7.58</v>
       </c>
-      <c r="D28" s="65" t="n">
+      <c r="D28" s="106" t="n">
         <v>8.37</v>
       </c>
-      <c r="E28" s="65" t="n">
+      <c r="E28" s="106" t="n">
         <v>8.27</v>
       </c>
-      <c r="F28" s="103" t="n">
+      <c r="F28" s="115" t="n">
         <v>8.4</v>
       </c>
-      <c r="G28" s="65" t="n">
+      <c r="G28" s="106" t="n">
         <v>8.47</v>
       </c>
-      <c r="H28" s="65" t="n">
+      <c r="H28" s="106" t="n">
         <v>8.52</v>
       </c>
-      <c r="I28" s="65" t="n">
+      <c r="I28" s="106" t="n">
         <v>8.14</v>
       </c>
-      <c r="J28" s="103" t="n">
+      <c r="J28" s="115" t="n">
         <v>7.4</v>
       </c>
-      <c r="K28" s="65" t="n">
+      <c r="K28" s="106" t="n">
         <v>7.04</v>
       </c>
-      <c r="L28" s="65" t="n">
+      <c r="L28" s="106" t="n">
         <v>6.81</v>
       </c>
-      <c r="M28" s="65" t="n">
+      <c r="M28" s="106" t="n">
         <v>6.77</v>
       </c>
-      <c r="N28" s="65" t="n">
+      <c r="N28" s="106" t="n">
         <v>5.31</v>
       </c>
       <c r="O28" s="14"/>
@@ -26701,307 +26780,307 @@
       <c r="B29" s="14" t="s">
         <v>571</v>
       </c>
-      <c r="C29" s="65" t="n">
+      <c r="C29" s="106" t="n">
         <v>6.08</v>
       </c>
-      <c r="D29" s="65" t="n">
+      <c r="D29" s="106" t="n">
         <v>7.74</v>
       </c>
-      <c r="E29" s="65" t="n">
+      <c r="E29" s="106" t="n">
         <v>11.7</v>
       </c>
-      <c r="F29" s="65" t="n">
+      <c r="F29" s="106" t="n">
         <v>10.1</v>
       </c>
-      <c r="G29" s="65" t="n">
+      <c r="G29" s="106" t="n">
         <v>9.96</v>
       </c>
-      <c r="H29" s="65" t="n">
+      <c r="H29" s="106" t="n">
         <v>10.7</v>
       </c>
-      <c r="I29" s="68" t="n">
+      <c r="I29" s="113" t="n">
         <v>11</v>
       </c>
-      <c r="J29" s="65" t="n">
+      <c r="J29" s="106" t="n">
         <v>9.67</v>
       </c>
-      <c r="K29" s="65" t="n">
+      <c r="K29" s="106" t="n">
         <v>12.3</v>
       </c>
-      <c r="L29" s="65" t="n">
+      <c r="L29" s="106" t="n">
         <v>6.02</v>
       </c>
-      <c r="M29" s="65" t="n">
+      <c r="M29" s="106" t="n">
         <v>5.18</v>
       </c>
-      <c r="N29" s="65" t="n">
+      <c r="N29" s="106" t="n">
         <v>4.78</v>
       </c>
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
       <c r="Q29" s="29"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="69" t="n">
+    <row r="30" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="76" t="n">
         <v>43007</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="73" t="s">
         <v>572</v>
       </c>
-      <c r="C30" s="39" t="n">
+      <c r="C30" s="116" t="n">
         <v>1.73</v>
       </c>
-      <c r="D30" s="39" t="n">
+      <c r="D30" s="116" t="n">
         <v>23.1</v>
       </c>
-      <c r="E30" s="39" t="n">
+      <c r="E30" s="116" t="n">
         <v>4.67</v>
       </c>
-      <c r="F30" s="39" t="n">
+      <c r="F30" s="116" t="n">
         <v>4.19</v>
       </c>
-      <c r="G30" s="39" t="n">
+      <c r="G30" s="116" t="n">
         <v>4.88</v>
       </c>
-      <c r="H30" s="72" t="n">
+      <c r="H30" s="117" t="n">
         <v>3.79</v>
       </c>
-      <c r="I30" s="22" t="n">
+      <c r="I30" s="118" t="n">
         <v>2.18</v>
       </c>
-      <c r="J30" s="25" t="n">
+      <c r="J30" s="73" t="n">
         <v>2.12</v>
       </c>
-      <c r="K30" s="39" t="n">
+      <c r="K30" s="116" t="n">
         <v>1.73</v>
       </c>
-      <c r="L30" s="39" t="n">
+      <c r="L30" s="116" t="n">
         <v>1.9</v>
       </c>
-      <c r="M30" s="39" t="n">
+      <c r="M30" s="116" t="n">
         <v>2.33</v>
       </c>
-      <c r="N30" s="39" t="n">
+      <c r="N30" s="116" t="n">
         <v>1.36</v>
       </c>
-      <c r="O30" s="39"/>
-      <c r="P30" s="72"/>
-      <c r="Q30" s="22"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="18" t="n">
+      <c r="O30" s="116"/>
+      <c r="P30" s="117"/>
+      <c r="Q30" s="118"/>
+    </row>
+    <row r="31" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="72" t="n">
         <v>42895</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="73" t="s">
         <v>573</v>
       </c>
-      <c r="C31" s="65" t="n">
+      <c r="C31" s="67" t="n">
         <v>2.56</v>
       </c>
-      <c r="D31" s="65" t="n">
+      <c r="D31" s="67" t="n">
         <v>3.31</v>
       </c>
-      <c r="E31" s="65" t="n">
+      <c r="E31" s="67" t="n">
         <v>4.24</v>
       </c>
-      <c r="F31" s="65" t="n">
+      <c r="F31" s="67" t="n">
         <v>10.5</v>
       </c>
-      <c r="G31" s="65" t="n">
+      <c r="G31" s="67" t="n">
         <v>13.9</v>
       </c>
-      <c r="H31" s="65" t="n">
+      <c r="H31" s="67" t="n">
         <v>14.9</v>
       </c>
-      <c r="I31" s="65" t="n">
+      <c r="I31" s="67" t="n">
         <v>17.6</v>
       </c>
-      <c r="J31" s="65" t="n">
+      <c r="J31" s="67" t="n">
         <v>12.7</v>
       </c>
-      <c r="K31" s="65" t="n">
+      <c r="K31" s="67" t="n">
         <v>19.9</v>
       </c>
-      <c r="L31" s="65" t="n">
+      <c r="L31" s="67" t="n">
         <v>21.6</v>
       </c>
-      <c r="M31" s="65" t="n">
+      <c r="M31" s="67" t="n">
         <v>4.21</v>
       </c>
-      <c r="N31" s="65" t="n">
+      <c r="N31" s="67" t="n">
         <v>2.03</v>
       </c>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="29"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28" t="n">
+      <c r="O31" s="66"/>
+      <c r="P31" s="66"/>
+      <c r="Q31" s="70"/>
+    </row>
+    <row r="32" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="65" t="n">
         <v>42860</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="73" t="s">
         <v>574</v>
       </c>
-      <c r="C32" s="81" t="n">
+      <c r="C32" s="119" t="n">
         <v>5.54</v>
       </c>
-      <c r="D32" s="81" t="n">
+      <c r="D32" s="119" t="n">
         <v>3.96</v>
       </c>
-      <c r="E32" s="81" t="n">
+      <c r="E32" s="119" t="n">
         <v>3.06</v>
       </c>
-      <c r="F32" s="20" t="n">
+      <c r="F32" s="120" t="n">
         <v>12.5</v>
       </c>
-      <c r="G32" s="20" t="n">
+      <c r="G32" s="120" t="n">
         <v>26.9</v>
       </c>
-      <c r="H32" s="20" t="n">
+      <c r="H32" s="120" t="n">
         <v>14.2</v>
       </c>
-      <c r="I32" s="20" t="n">
+      <c r="I32" s="120" t="n">
         <v>13.2</v>
       </c>
-      <c r="J32" s="20" t="n">
+      <c r="J32" s="120" t="n">
         <v>30.9</v>
       </c>
-      <c r="K32" s="20" t="n">
+      <c r="K32" s="120" t="n">
         <v>20.6</v>
       </c>
-      <c r="L32" s="81" t="n">
+      <c r="L32" s="119" t="n">
         <v>5.13</v>
       </c>
-      <c r="M32" s="81" t="n">
+      <c r="M32" s="119" t="n">
         <v>9.49</v>
       </c>
-      <c r="N32" s="81" t="n">
+      <c r="N32" s="119" t="n">
         <v>2.79</v>
       </c>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28" t="n">
+      <c r="O32" s="75"/>
+      <c r="P32" s="75"/>
+      <c r="Q32" s="75"/>
+    </row>
+    <row r="33" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="65" t="n">
         <v>42948</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="73" t="s">
         <v>574</v>
       </c>
-      <c r="C33" s="20" t="n">
+      <c r="C33" s="120" t="n">
         <v>13.1</v>
       </c>
-      <c r="D33" s="104" t="n">
+      <c r="D33" s="121" t="n">
         <v>3</v>
       </c>
-      <c r="E33" s="81" t="n">
+      <c r="E33" s="119" t="n">
         <v>3.05</v>
       </c>
-      <c r="F33" s="81" t="n">
+      <c r="F33" s="119" t="n">
         <v>3.84</v>
       </c>
-      <c r="G33" s="81" t="n">
+      <c r="G33" s="119" t="n">
         <v>6.53</v>
       </c>
-      <c r="H33" s="81" t="n">
+      <c r="H33" s="119" t="n">
         <v>8.34</v>
       </c>
-      <c r="I33" s="20" t="n">
+      <c r="I33" s="120" t="n">
         <v>11.6</v>
       </c>
-      <c r="J33" s="81" t="n">
+      <c r="J33" s="119" t="n">
         <v>9.71</v>
       </c>
-      <c r="K33" s="81" t="n">
+      <c r="K33" s="119" t="n">
         <v>9.46</v>
       </c>
-      <c r="L33" s="20" t="n">
+      <c r="L33" s="120" t="n">
         <v>14.4</v>
       </c>
-      <c r="M33" s="20" t="n">
+      <c r="M33" s="120" t="n">
         <v>8.2</v>
       </c>
-      <c r="N33" s="81" t="n">
+      <c r="N33" s="119" t="n">
         <v>3.1</v>
       </c>
-      <c r="O33" s="29" t="n">
+      <c r="O33" s="70" t="n">
         <v>3.16</v>
       </c>
-      <c r="P33" s="29" t="n">
+      <c r="P33" s="70" t="n">
         <v>2.92</v>
       </c>
-      <c r="Q33" s="29" t="n">
+      <c r="Q33" s="70" t="n">
         <v>2.65</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18" t="n">
+    <row r="34" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="72" t="n">
         <v>42987</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="66" t="s">
         <v>575</v>
       </c>
-      <c r="C34" s="103" t="n">
+      <c r="C34" s="122" t="n">
         <v>5.12</v>
       </c>
-      <c r="D34" s="81" t="n">
+      <c r="D34" s="119" t="n">
         <v>6.39</v>
       </c>
-      <c r="E34" s="81" t="n">
+      <c r="E34" s="119" t="n">
         <v>6.69</v>
       </c>
-      <c r="F34" s="81" t="n">
+      <c r="F34" s="119" t="n">
         <v>7.95</v>
       </c>
-      <c r="G34" s="29" t="n">
+      <c r="G34" s="70" t="n">
         <v>7.27</v>
       </c>
-      <c r="H34" s="29" t="n">
+      <c r="H34" s="70" t="n">
         <v>6.66</v>
       </c>
-      <c r="I34" s="29" t="n">
+      <c r="I34" s="70" t="n">
         <v>6.45</v>
       </c>
-      <c r="J34" s="29" t="n">
+      <c r="J34" s="70" t="n">
         <v>6.6</v>
       </c>
-      <c r="K34" s="29" t="n">
+      <c r="K34" s="70" t="n">
         <v>6.48</v>
       </c>
-      <c r="L34" s="29" t="n">
+      <c r="L34" s="70" t="n">
         <v>6.17</v>
       </c>
-      <c r="M34" s="29" t="n">
+      <c r="M34" s="70" t="n">
         <v>5.51</v>
       </c>
-      <c r="N34" s="29" t="n">
+      <c r="N34" s="70" t="n">
         <v>5</v>
       </c>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="29"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="66"/>
+      <c r="Q34" s="70"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="55" t="s">
         <v>529</v>
       </c>
-      <c r="B35" s="105"/>
-      <c r="C35" s="105"/>
-      <c r="D35" s="105"/>
-      <c r="E35" s="105"/>
-      <c r="F35" s="105"/>
-      <c r="G35" s="105"/>
-      <c r="H35" s="105"/>
-      <c r="I35" s="105"/>
-      <c r="J35" s="105"/>
-      <c r="K35" s="105"/>
-      <c r="L35" s="105"/>
-      <c r="M35" s="105"/>
-      <c r="N35" s="105"/>
-      <c r="O35" s="105"/>
-      <c r="P35" s="105"/>
-      <c r="Q35" s="105"/>
+      <c r="B35" s="123"/>
+      <c r="C35" s="123"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="123"/>
+      <c r="I35" s="123"/>
+      <c r="J35" s="123"/>
+      <c r="K35" s="123"/>
+      <c r="L35" s="123"/>
+      <c r="M35" s="123"/>
+      <c r="N35" s="123"/>
+      <c r="O35" s="123"/>
+      <c r="P35" s="123"/>
+      <c r="Q35" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -27030,7 +27109,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>#ref!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
working on methods for tf_nn file
</commit_message>
<xml_diff>
--- a/wq_study_results.xlsx
+++ b/wq_study_results.xlsx
@@ -1698,7 +1698,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">26XX N. Drake Ave.</t>
     </r>
@@ -1709,7 +1708,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Site 2</t>
     </r>
@@ -1723,7 +1721,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">28XX N. Christiana Ave. </t>
     </r>
@@ -1733,7 +1730,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Site 2</t>
     </r>
@@ -1751,7 +1747,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">32XX N. Nagle Ave. </t>
     </r>
@@ -1762,7 +1757,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Site 3</t>
     </r>
@@ -1777,7 +1771,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">34XX S. Marshfield Ave. </t>
     </r>
@@ -1788,7 +1781,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Site 2</t>
     </r>
@@ -1799,7 +1791,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">36XX S. Paulina St.</t>
     </r>
@@ -1810,7 +1801,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Site 2</t>
     </r>
@@ -1821,7 +1811,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">37XX N. Whipple St. </t>
     </r>
@@ -1831,7 +1820,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Site 1</t>
     </r>
@@ -1842,7 +1830,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">38XX N. Whipple St. </t>
     </r>
@@ -1852,7 +1839,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Site 3</t>
     </r>
@@ -1864,7 +1850,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">39XX N. Whipple St. </t>
     </r>
@@ -1875,7 +1860,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Site 1</t>
     </r>
@@ -1892,7 +1876,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">45XX N. Albany Ave.</t>
     </r>
@@ -1902,7 +1885,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Site 2</t>
     </r>
@@ -1913,7 +1895,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">45XX N. Whipple St. </t>
     </r>
@@ -1924,7 +1905,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Site 4</t>
     </r>
@@ -1944,7 +1924,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">66XX S. Kilpatrick Ave. </t>
     </r>
@@ -1955,7 +1934,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Site 3</t>
     </r>
@@ -1987,7 +1965,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2009,14 +1986,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2025,7 +2000,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2033,40 +2007,34 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2075,7 +2043,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2207,7 +2174,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="119">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2532,146 +2499,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2684,6 +2511,42 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2692,12 +2555,96 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2717,6 +2664,8 @@
   <dxfs count="28">
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <family val="2"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2726,6 +2675,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2733,6 +2687,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2740,6 +2699,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2747,6 +2711,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2754,6 +2723,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2761,6 +2735,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2768,6 +2747,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2775,6 +2759,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2782,6 +2771,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2789,6 +2783,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2796,6 +2795,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2803,6 +2807,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2810,6 +2819,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2817,6 +2831,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2824,6 +2843,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2831,6 +2855,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2838,6 +2867,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2845,6 +2879,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2852,6 +2891,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2859,6 +2903,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2866,6 +2915,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2873,6 +2927,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2880,6 +2939,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2887,6 +2951,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2894,6 +2963,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2901,6 +2975,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -2908,6 +2987,11 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
@@ -3028,8 +3112,8 @@
   </sheetPr>
   <dimension ref="A1:Q851"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B595" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A617" activeCellId="0" sqref="A617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -25435,7 +25519,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25691,1134 +25775,1134 @@
       <c r="P6" s="78"/>
       <c r="Q6" s="79"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="81" t="n">
+    <row r="7" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="76" t="n">
         <v>43056</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="73" t="s">
         <v>549</v>
       </c>
-      <c r="C7" s="39" t="n">
+      <c r="C7" s="81" t="n">
         <v>7.68</v>
       </c>
-      <c r="D7" s="39" t="n">
+      <c r="D7" s="81" t="n">
         <v>7.9</v>
       </c>
-      <c r="E7" s="39" t="n">
+      <c r="E7" s="81" t="n">
         <v>16.1</v>
       </c>
-      <c r="F7" s="39" t="n">
+      <c r="F7" s="81" t="n">
         <v>19.9</v>
       </c>
-      <c r="G7" s="39" t="n">
+      <c r="G7" s="81" t="n">
         <v>19.3</v>
       </c>
       <c r="H7" s="82" t="n">
         <v>20.8</v>
       </c>
-      <c r="I7" s="22" t="n">
+      <c r="I7" s="83" t="n">
         <v>63.1</v>
       </c>
-      <c r="J7" s="25" t="n">
+      <c r="J7" s="73" t="n">
         <v>26</v>
       </c>
-      <c r="K7" s="39" t="n">
+      <c r="K7" s="81" t="n">
         <v>26.2</v>
       </c>
-      <c r="L7" s="39" t="n">
+      <c r="L7" s="81" t="n">
         <v>27.4</v>
       </c>
-      <c r="M7" s="39" t="n">
+      <c r="M7" s="81" t="n">
         <v>21</v>
       </c>
-      <c r="N7" s="39" t="n">
+      <c r="N7" s="81" t="n">
         <v>8.7</v>
       </c>
-      <c r="O7" s="83"/>
+      <c r="O7" s="84"/>
       <c r="P7" s="82"/>
-      <c r="Q7" s="22"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="81" t="n">
+      <c r="Q7" s="83"/>
+    </row>
+    <row r="8" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="76" t="n">
         <v>43105</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="80" t="s">
         <v>550</v>
       </c>
-      <c r="C8" s="84" t="n">
+      <c r="C8" s="85" t="n">
         <v>4.46</v>
       </c>
-      <c r="D8" s="85" t="n">
+      <c r="D8" s="86" t="n">
         <v>2.99</v>
       </c>
-      <c r="E8" s="85" t="n">
+      <c r="E8" s="86" t="n">
         <v>3.48</v>
       </c>
-      <c r="F8" s="85" t="n">
+      <c r="F8" s="86" t="n">
         <v>5.18</v>
       </c>
-      <c r="G8" s="86" t="n">
+      <c r="G8" s="87" t="n">
         <v>4.56</v>
       </c>
-      <c r="H8" s="86" t="n">
+      <c r="H8" s="87" t="n">
         <v>4.52</v>
       </c>
-      <c r="I8" s="86" t="n">
+      <c r="I8" s="87" t="n">
         <v>5.94</v>
       </c>
-      <c r="J8" s="85" t="n">
+      <c r="J8" s="86" t="n">
         <v>6.8</v>
       </c>
-      <c r="K8" s="86" t="n">
+      <c r="K8" s="87" t="n">
         <v>6.71</v>
       </c>
-      <c r="L8" s="86" t="n">
+      <c r="L8" s="87" t="n">
         <v>6.69</v>
       </c>
-      <c r="M8" s="86" t="n">
+      <c r="M8" s="87" t="n">
         <v>2.65</v>
       </c>
-      <c r="N8" s="86" t="n">
+      <c r="N8" s="87" t="n">
         <v>1.74</v>
       </c>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="29"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="n">
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="70"/>
+    </row>
+    <row r="9" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="72" t="n">
         <v>42829</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="73" t="s">
         <v>551</v>
       </c>
-      <c r="C9" s="87" t="n">
+      <c r="C9" s="89" t="n">
         <v>23</v>
       </c>
-      <c r="D9" s="88" t="n">
+      <c r="D9" s="90" t="n">
         <v>5.23</v>
       </c>
-      <c r="E9" s="88" t="n">
+      <c r="E9" s="90" t="n">
         <v>4.29</v>
       </c>
-      <c r="F9" s="88" t="n">
+      <c r="F9" s="90" t="n">
         <v>4.56</v>
       </c>
-      <c r="G9" s="88" t="n">
+      <c r="G9" s="90" t="n">
         <v>4.53</v>
       </c>
-      <c r="H9" s="88" t="n">
+      <c r="H9" s="90" t="n">
         <v>3.48</v>
       </c>
-      <c r="I9" s="88" t="n">
+      <c r="I9" s="90" t="n">
         <v>9.66</v>
       </c>
-      <c r="J9" s="88" t="n">
+      <c r="J9" s="90" t="n">
         <v>8.68</v>
       </c>
-      <c r="K9" s="88" t="n">
+      <c r="K9" s="90" t="n">
         <v>8.57</v>
       </c>
-      <c r="L9" s="88" t="n">
+      <c r="L9" s="90" t="n">
         <v>6.81</v>
       </c>
-      <c r="M9" s="88" t="n">
+      <c r="M9" s="90" t="n">
         <v>3.92</v>
       </c>
-      <c r="N9" s="88" t="n">
+      <c r="N9" s="90" t="n">
         <v>3.32</v>
       </c>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="89"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28" t="n">
+      <c r="O9" s="88"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="91"/>
+    </row>
+    <row r="10" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="65" t="n">
         <v>42676</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="92" t="s">
         <v>552</v>
       </c>
-      <c r="C10" s="91" t="n">
+      <c r="C10" s="93" t="n">
         <v>5.07</v>
       </c>
-      <c r="D10" s="91" t="n">
+      <c r="D10" s="93" t="n">
         <v>5.72</v>
       </c>
-      <c r="E10" s="91" t="n">
+      <c r="E10" s="93" t="n">
         <v>3.06</v>
       </c>
-      <c r="F10" s="91" t="n">
+      <c r="F10" s="93" t="n">
         <v>2.65</v>
       </c>
-      <c r="G10" s="91" t="n">
+      <c r="G10" s="93" t="n">
         <v>6.3</v>
       </c>
-      <c r="H10" s="20" t="n">
+      <c r="H10" s="94" t="n">
         <v>11.9</v>
       </c>
-      <c r="I10" s="20" t="n">
+      <c r="I10" s="94" t="n">
         <v>25</v>
       </c>
-      <c r="J10" s="20" t="n">
+      <c r="J10" s="94" t="n">
         <v>24</v>
       </c>
-      <c r="K10" s="20" t="n">
+      <c r="K10" s="94" t="n">
         <v>12.4</v>
       </c>
-      <c r="L10" s="91" t="n">
+      <c r="L10" s="93" t="n">
         <v>5.7</v>
       </c>
-      <c r="M10" s="91" t="n">
+      <c r="M10" s="93" t="n">
         <v>4.22</v>
       </c>
-      <c r="N10" s="91" t="n">
+      <c r="N10" s="93" t="n">
         <v>3.15</v>
       </c>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="29"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="92" t="n">
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="70"/>
+    </row>
+    <row r="11" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="95" t="n">
         <v>42951</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="87" t="s">
         <v>553</v>
       </c>
-      <c r="C11" s="84" t="n">
+      <c r="C11" s="85" t="n">
         <v>1.61</v>
       </c>
-      <c r="D11" s="93" t="n">
+      <c r="D11" s="96" t="n">
         <v>2.1</v>
       </c>
-      <c r="E11" s="93" t="n">
+      <c r="E11" s="96" t="n">
         <v>1.65</v>
       </c>
-      <c r="F11" s="94" t="s">
+      <c r="F11" s="97" t="s">
         <v>554</v>
       </c>
-      <c r="G11" s="95" t="s">
+      <c r="G11" s="98" t="s">
         <v>554</v>
       </c>
-      <c r="H11" s="95" t="s">
+      <c r="H11" s="98" t="s">
         <v>554</v>
       </c>
-      <c r="I11" s="95" t="s">
+      <c r="I11" s="98" t="s">
         <v>554</v>
       </c>
-      <c r="J11" s="95" t="s">
+      <c r="J11" s="98" t="s">
         <v>554</v>
       </c>
-      <c r="K11" s="95" t="s">
+      <c r="K11" s="98" t="s">
         <v>554</v>
       </c>
-      <c r="L11" s="95" t="s">
+      <c r="L11" s="98" t="s">
         <v>554</v>
       </c>
-      <c r="M11" s="95" t="s">
+      <c r="M11" s="98" t="s">
         <v>554</v>
       </c>
-      <c r="N11" s="95" t="s">
+      <c r="N11" s="98" t="s">
         <v>554</v>
       </c>
-      <c r="O11" s="96" t="s">
+      <c r="O11" s="99" t="s">
         <v>554</v>
       </c>
-      <c r="P11" s="96" t="s">
+      <c r="P11" s="99" t="s">
         <v>554</v>
       </c>
-      <c r="Q11" s="96" t="s">
+      <c r="Q11" s="99" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="97" t="n">
+    <row r="12" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="100" t="n">
         <v>42832</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="80" t="s">
         <v>555</v>
       </c>
-      <c r="C12" s="87" t="n">
+      <c r="C12" s="89" t="n">
         <v>10.4</v>
       </c>
-      <c r="D12" s="87" t="n">
+      <c r="D12" s="89" t="n">
         <v>15.6</v>
       </c>
-      <c r="E12" s="87" t="n">
+      <c r="E12" s="89" t="n">
         <v>14.2</v>
       </c>
-      <c r="F12" s="87" t="n">
+      <c r="F12" s="89" t="n">
         <v>11.9</v>
       </c>
-      <c r="G12" s="88" t="n">
+      <c r="G12" s="90" t="n">
         <v>11.1</v>
       </c>
-      <c r="H12" s="88" t="n">
+      <c r="H12" s="90" t="n">
         <v>10.2</v>
       </c>
-      <c r="I12" s="88" t="n">
+      <c r="I12" s="90" t="n">
         <v>9.54</v>
       </c>
-      <c r="J12" s="88" t="n">
+      <c r="J12" s="90" t="n">
         <v>8.5</v>
       </c>
-      <c r="K12" s="88" t="n">
+      <c r="K12" s="90" t="n">
         <v>8.41</v>
       </c>
-      <c r="L12" s="88" t="n">
+      <c r="L12" s="90" t="n">
         <v>6.53</v>
       </c>
-      <c r="M12" s="88" t="n">
+      <c r="M12" s="90" t="n">
         <v>5.33</v>
       </c>
-      <c r="N12" s="88" t="n">
+      <c r="N12" s="90" t="n">
         <v>4.94</v>
       </c>
-      <c r="O12" s="98" t="n">
+      <c r="O12" s="101" t="n">
         <v>4.6</v>
       </c>
-      <c r="P12" s="51" t="n">
+      <c r="P12" s="88" t="n">
         <v>4.49</v>
       </c>
-      <c r="Q12" s="89" t="n">
+      <c r="Q12" s="91" t="n">
         <v>4.32</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28" t="n">
+    <row r="13" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="65" t="n">
         <v>42797</v>
       </c>
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="102" t="s">
         <v>556</v>
       </c>
-      <c r="C13" s="88" t="n">
+      <c r="C13" s="90" t="n">
         <v>4.07</v>
       </c>
-      <c r="D13" s="88" t="n">
+      <c r="D13" s="90" t="n">
         <v>3.18</v>
       </c>
-      <c r="E13" s="88" t="n">
+      <c r="E13" s="90" t="n">
         <v>3.16</v>
       </c>
-      <c r="F13" s="88" t="n">
+      <c r="F13" s="90" t="n">
         <v>2.4</v>
       </c>
-      <c r="G13" s="88" t="n">
+      <c r="G13" s="90" t="n">
         <v>3.44</v>
       </c>
-      <c r="H13" s="88" t="n">
+      <c r="H13" s="90" t="n">
         <v>3.92</v>
       </c>
-      <c r="I13" s="88" t="n">
+      <c r="I13" s="90" t="n">
         <v>2.6</v>
       </c>
-      <c r="J13" s="88" t="n">
+      <c r="J13" s="90" t="n">
         <v>4.04</v>
       </c>
-      <c r="K13" s="88" t="n">
+      <c r="K13" s="90" t="n">
         <v>2.73</v>
       </c>
-      <c r="L13" s="88" t="n">
+      <c r="L13" s="90" t="n">
         <v>5.05</v>
       </c>
-      <c r="M13" s="88" t="n">
+      <c r="M13" s="90" t="n">
         <v>3.05</v>
       </c>
-      <c r="N13" s="88" t="n">
+      <c r="N13" s="90" t="n">
         <v>1.36</v>
       </c>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="89"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="92" t="n">
+      <c r="O13" s="88"/>
+      <c r="P13" s="88"/>
+      <c r="Q13" s="91"/>
+    </row>
+    <row r="14" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="95" t="n">
         <v>42949</v>
       </c>
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="103" t="s">
         <v>557</v>
       </c>
-      <c r="C14" s="91" t="n">
+      <c r="C14" s="93" t="n">
         <v>9.55</v>
       </c>
-      <c r="D14" s="91" t="n">
+      <c r="D14" s="93" t="n">
         <v>9.54</v>
       </c>
-      <c r="E14" s="91" t="n">
+      <c r="E14" s="93" t="n">
         <v>9.15</v>
       </c>
-      <c r="F14" s="91" t="n">
+      <c r="F14" s="93" t="n">
         <v>9.45</v>
       </c>
-      <c r="G14" s="20" t="n">
+      <c r="G14" s="94" t="n">
         <v>19.1</v>
       </c>
-      <c r="H14" s="20" t="n">
+      <c r="H14" s="94" t="n">
         <v>43.9</v>
       </c>
-      <c r="I14" s="20" t="n">
+      <c r="I14" s="94" t="n">
         <v>35.3</v>
       </c>
-      <c r="J14" s="20" t="n">
+      <c r="J14" s="94" t="n">
         <v>24.9</v>
       </c>
-      <c r="K14" s="20" t="n">
+      <c r="K14" s="94" t="n">
         <v>23.1</v>
       </c>
-      <c r="L14" s="20" t="n">
+      <c r="L14" s="94" t="n">
         <v>22.4</v>
       </c>
-      <c r="M14" s="20" t="n">
+      <c r="M14" s="94" t="n">
         <v>23.2</v>
       </c>
-      <c r="N14" s="91" t="n">
+      <c r="N14" s="93" t="n">
         <v>8.76</v>
       </c>
-      <c r="O14" s="29" t="n">
+      <c r="O14" s="70" t="n">
         <v>8.37</v>
       </c>
-      <c r="P14" s="29" t="n">
+      <c r="P14" s="70" t="n">
         <v>7.1</v>
       </c>
-      <c r="Q14" s="29" t="n">
+      <c r="Q14" s="70" t="n">
         <v>6.86</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="92" t="n">
+    <row r="15" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="95" t="n">
         <v>42997</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="103" t="s">
         <v>558</v>
       </c>
-      <c r="C15" s="101" t="n">
+      <c r="C15" s="104" t="n">
         <v>6.31</v>
       </c>
-      <c r="D15" s="102" t="n">
+      <c r="D15" s="105" t="n">
         <v>8.05</v>
       </c>
-      <c r="E15" s="102" t="n">
+      <c r="E15" s="105" t="n">
         <v>7.46</v>
       </c>
-      <c r="F15" s="102" t="n">
+      <c r="F15" s="105" t="n">
         <v>8.4</v>
       </c>
-      <c r="G15" s="103" t="n">
+      <c r="G15" s="106" t="n">
         <v>11.2</v>
       </c>
-      <c r="H15" s="103" t="n">
+      <c r="H15" s="106" t="n">
         <v>14.1</v>
       </c>
-      <c r="I15" s="103" t="n">
+      <c r="I15" s="106" t="n">
         <v>15.7</v>
       </c>
-      <c r="J15" s="103" t="n">
+      <c r="J15" s="106" t="n">
         <v>15.6</v>
       </c>
-      <c r="K15" s="103" t="s">
+      <c r="K15" s="106" t="s">
         <v>559</v>
       </c>
-      <c r="L15" s="96" t="s">
+      <c r="L15" s="99" t="s">
         <v>559</v>
       </c>
-      <c r="M15" s="103" t="n">
+      <c r="M15" s="106" t="n">
         <v>15.2</v>
       </c>
-      <c r="N15" s="96" t="n">
+      <c r="N15" s="99" t="n">
         <v>27</v>
       </c>
-      <c r="O15" s="104" t="n">
+      <c r="O15" s="107" t="n">
         <v>4.99</v>
       </c>
-      <c r="P15" s="103" t="n">
+      <c r="P15" s="106" t="n">
         <v>4.15</v>
       </c>
-      <c r="Q15" s="102" t="n">
+      <c r="Q15" s="105" t="n">
         <v>4.01</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="n">
+    <row r="16" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65" t="n">
         <v>42926</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="66" t="s">
         <v>560</v>
       </c>
-      <c r="C16" s="105" t="n">
+      <c r="C16" s="108" t="n">
         <v>24</v>
       </c>
-      <c r="D16" s="105" t="n">
+      <c r="D16" s="108" t="n">
         <v>28.8</v>
       </c>
-      <c r="E16" s="105" t="n">
+      <c r="E16" s="108" t="n">
         <v>58.2</v>
       </c>
-      <c r="F16" s="105" t="n">
+      <c r="F16" s="108" t="n">
         <v>29</v>
       </c>
-      <c r="G16" s="105" t="n">
+      <c r="G16" s="108" t="n">
         <v>21.7</v>
       </c>
-      <c r="H16" s="105" t="n">
+      <c r="H16" s="108" t="n">
         <v>20.3</v>
       </c>
-      <c r="I16" s="105" t="n">
+      <c r="I16" s="108" t="n">
         <v>20.1</v>
       </c>
-      <c r="J16" s="105" t="n">
+      <c r="J16" s="108" t="n">
         <v>13.1</v>
       </c>
-      <c r="K16" s="105" t="n">
+      <c r="K16" s="108" t="n">
         <v>10.5</v>
       </c>
-      <c r="L16" s="105" t="n">
+      <c r="L16" s="108" t="n">
         <v>9.82</v>
       </c>
-      <c r="M16" s="105" t="n">
+      <c r="M16" s="108" t="n">
         <v>9.51</v>
       </c>
-      <c r="N16" s="105" t="n">
+      <c r="N16" s="108" t="n">
         <v>8.93</v>
       </c>
-      <c r="O16" s="106" t="n">
+      <c r="O16" s="67" t="n">
         <v>8.77</v>
       </c>
-      <c r="P16" s="106" t="n">
+      <c r="P16" s="67" t="n">
         <v>8.33</v>
       </c>
-      <c r="Q16" s="106" t="n">
+      <c r="Q16" s="67" t="n">
         <v>7.95</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28" t="n">
+    <row r="17" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="65" t="n">
         <v>42893</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="73" t="s">
         <v>561</v>
       </c>
-      <c r="C17" s="107" t="n">
+      <c r="C17" s="109" t="n">
         <v>6.19</v>
       </c>
-      <c r="D17" s="107" t="n">
+      <c r="D17" s="109" t="n">
         <v>2.55</v>
       </c>
-      <c r="E17" s="107" t="n">
+      <c r="E17" s="109" t="n">
         <v>4.78</v>
       </c>
-      <c r="F17" s="107" t="n">
+      <c r="F17" s="109" t="n">
         <v>2.27</v>
       </c>
-      <c r="G17" s="108" t="n">
+      <c r="G17" s="110" t="n">
         <v>2.3</v>
       </c>
-      <c r="H17" s="107" t="n">
+      <c r="H17" s="109" t="n">
         <v>2.58</v>
       </c>
-      <c r="I17" s="107" t="n">
+      <c r="I17" s="109" t="n">
         <v>4.33</v>
       </c>
-      <c r="J17" s="107" t="n">
+      <c r="J17" s="109" t="n">
         <v>2.22</v>
       </c>
-      <c r="K17" s="107" t="n">
+      <c r="K17" s="109" t="n">
         <v>2.13</v>
       </c>
-      <c r="L17" s="107" t="n">
+      <c r="L17" s="109" t="n">
         <v>2.13</v>
       </c>
-      <c r="M17" s="107" t="n">
+      <c r="M17" s="109" t="n">
         <v>1.96</v>
       </c>
-      <c r="N17" s="107" t="n">
+      <c r="N17" s="109" t="n">
         <v>1.91</v>
       </c>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="89"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="n">
+      <c r="O17" s="88"/>
+      <c r="P17" s="88"/>
+      <c r="Q17" s="91"/>
+    </row>
+    <row r="18" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="72" t="n">
         <v>42882</v>
       </c>
-      <c r="B18" s="109" t="s">
+      <c r="B18" s="111" t="s">
         <v>562</v>
       </c>
-      <c r="C18" s="107" t="n">
+      <c r="C18" s="109" t="n">
         <v>5.2</v>
       </c>
-      <c r="D18" s="107" t="n">
+      <c r="D18" s="109" t="n">
         <v>6.06</v>
       </c>
-      <c r="E18" s="107" t="n">
+      <c r="E18" s="109" t="n">
         <v>5.11</v>
       </c>
-      <c r="F18" s="107" t="n">
+      <c r="F18" s="109" t="n">
         <v>7.11</v>
       </c>
-      <c r="G18" s="107" t="n">
+      <c r="G18" s="109" t="n">
         <v>6.05</v>
       </c>
-      <c r="H18" s="107" t="n">
+      <c r="H18" s="109" t="n">
         <v>4.51</v>
       </c>
-      <c r="I18" s="107" t="n">
+      <c r="I18" s="109" t="n">
         <v>4.96</v>
       </c>
-      <c r="J18" s="107" t="n">
+      <c r="J18" s="109" t="n">
         <v>3.55</v>
       </c>
-      <c r="K18" s="107" t="n">
+      <c r="K18" s="109" t="n">
         <v>3.49</v>
       </c>
-      <c r="L18" s="107" t="n">
+      <c r="L18" s="109" t="n">
         <v>2.22</v>
       </c>
-      <c r="M18" s="108" t="n">
+      <c r="M18" s="110" t="n">
         <v>2</v>
       </c>
-      <c r="N18" s="107" t="n">
+      <c r="N18" s="109" t="n">
         <v>1.57</v>
       </c>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="29"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="110" t="n">
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="70"/>
+    </row>
+    <row r="19" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="112" t="n">
         <v>42882</v>
       </c>
-      <c r="B19" s="111" t="s">
+      <c r="B19" s="113" t="s">
         <v>563</v>
       </c>
-      <c r="C19" s="107" t="n">
+      <c r="C19" s="109" t="n">
         <v>13.9</v>
       </c>
-      <c r="D19" s="107" t="n">
+      <c r="D19" s="109" t="n">
         <v>23.1</v>
       </c>
-      <c r="E19" s="107" t="n">
+      <c r="E19" s="109" t="n">
         <v>39.8</v>
       </c>
-      <c r="F19" s="107" t="n">
+      <c r="F19" s="109" t="n">
         <v>26.7</v>
       </c>
-      <c r="G19" s="107" t="n">
+      <c r="G19" s="109" t="n">
         <v>27</v>
       </c>
-      <c r="H19" s="107" t="n">
+      <c r="H19" s="109" t="n">
         <v>25.3</v>
       </c>
-      <c r="I19" s="107" t="n">
+      <c r="I19" s="109" t="n">
         <v>24.9</v>
       </c>
-      <c r="J19" s="107" t="n">
+      <c r="J19" s="109" t="n">
         <v>24.7</v>
       </c>
-      <c r="K19" s="107" t="n">
+      <c r="K19" s="109" t="n">
         <v>33.1</v>
       </c>
-      <c r="L19" s="107" t="n">
+      <c r="L19" s="109" t="n">
         <v>17.4</v>
       </c>
-      <c r="M19" s="107" t="n">
+      <c r="M19" s="109" t="n">
         <v>6.18</v>
       </c>
-      <c r="N19" s="107" t="n">
+      <c r="N19" s="109" t="n">
         <v>5.3</v>
       </c>
-      <c r="O19" s="104"/>
-      <c r="P19" s="103"/>
-      <c r="Q19" s="102"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18" t="n">
+      <c r="O19" s="107"/>
+      <c r="P19" s="106"/>
+      <c r="Q19" s="105"/>
+    </row>
+    <row r="20" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="72" t="n">
         <v>42957</v>
       </c>
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="111" t="s">
         <v>563</v>
       </c>
-      <c r="C20" s="106" t="n">
+      <c r="C20" s="67" t="n">
         <v>14.3</v>
       </c>
-      <c r="D20" s="106" t="n">
+      <c r="D20" s="67" t="n">
         <v>21.7</v>
       </c>
-      <c r="E20" s="106" t="n">
+      <c r="E20" s="67" t="n">
         <v>28.2</v>
       </c>
-      <c r="F20" s="106" t="n">
+      <c r="F20" s="67" t="n">
         <v>29.6</v>
       </c>
-      <c r="G20" s="106" t="n">
+      <c r="G20" s="67" t="n">
         <v>30.5</v>
       </c>
-      <c r="H20" s="106" t="n">
+      <c r="H20" s="67" t="n">
         <v>30</v>
       </c>
-      <c r="I20" s="106" t="n">
+      <c r="I20" s="67" t="n">
         <v>33.6</v>
       </c>
-      <c r="J20" s="106" t="n">
+      <c r="J20" s="67" t="n">
         <v>38.6</v>
       </c>
-      <c r="K20" s="106" t="n">
+      <c r="K20" s="67" t="n">
         <v>34.8</v>
       </c>
-      <c r="L20" s="106" t="n">
+      <c r="L20" s="67" t="n">
         <v>32.1</v>
       </c>
-      <c r="M20" s="106" t="n">
+      <c r="M20" s="67" t="n">
         <v>10.4</v>
       </c>
-      <c r="N20" s="106" t="n">
+      <c r="N20" s="67" t="n">
         <v>8.32</v>
       </c>
-      <c r="O20" s="112" t="n">
+      <c r="O20" s="114" t="n">
         <v>8.04</v>
       </c>
-      <c r="P20" s="107" t="n">
+      <c r="P20" s="109" t="n">
         <v>7.87</v>
       </c>
-      <c r="Q20" s="107" t="n">
+      <c r="Q20" s="109" t="n">
         <v>7.61</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="n">
+    <row r="21" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="65" t="n">
         <v>42893</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="66" t="s">
         <v>564</v>
       </c>
-      <c r="C21" s="106" t="n">
+      <c r="C21" s="67" t="n">
         <v>177</v>
       </c>
-      <c r="D21" s="106" t="n">
+      <c r="D21" s="67" t="n">
         <v>93.4</v>
       </c>
-      <c r="E21" s="106" t="n">
+      <c r="E21" s="67" t="n">
         <v>123</v>
       </c>
-      <c r="F21" s="106" t="n">
+      <c r="F21" s="67" t="n">
         <v>110</v>
       </c>
-      <c r="G21" s="106" t="n">
+      <c r="G21" s="67" t="n">
         <v>84.1</v>
       </c>
-      <c r="H21" s="106" t="n">
+      <c r="H21" s="67" t="n">
         <v>70.9</v>
       </c>
-      <c r="I21" s="106" t="n">
+      <c r="I21" s="67" t="n">
         <v>41.5</v>
       </c>
-      <c r="J21" s="106" t="n">
+      <c r="J21" s="67" t="n">
         <v>22.7</v>
       </c>
-      <c r="K21" s="106" t="n">
+      <c r="K21" s="67" t="n">
         <v>42.5</v>
       </c>
-      <c r="L21" s="106" t="n">
+      <c r="L21" s="67" t="n">
         <v>52.9</v>
       </c>
-      <c r="M21" s="106" t="n">
+      <c r="M21" s="67" t="n">
         <v>9.93</v>
       </c>
-      <c r="N21" s="106" t="n">
+      <c r="N21" s="67" t="n">
         <v>7.82</v>
       </c>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="29"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="81" t="n">
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="70"/>
+    </row>
+    <row r="22" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="76" t="n">
         <v>43061</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="73" t="s">
         <v>565</v>
       </c>
-      <c r="C22" s="113" t="n">
+      <c r="C22" s="74" t="n">
         <v>12.7</v>
       </c>
-      <c r="D22" s="31" t="n">
+      <c r="D22" s="75" t="n">
         <v>12.5</v>
       </c>
-      <c r="E22" s="31" t="n">
+      <c r="E22" s="75" t="n">
         <v>11.6</v>
       </c>
-      <c r="F22" s="31" t="n">
+      <c r="F22" s="75" t="n">
         <v>11.5</v>
       </c>
-      <c r="G22" s="14" t="n">
+      <c r="G22" s="66" t="n">
         <v>16.9</v>
       </c>
-      <c r="H22" s="14" t="n">
+      <c r="H22" s="66" t="n">
         <v>23.1</v>
       </c>
-      <c r="I22" s="14" t="n">
+      <c r="I22" s="66" t="n">
         <v>24.6</v>
       </c>
-      <c r="J22" s="14" t="n">
+      <c r="J22" s="66" t="n">
         <v>23.7</v>
       </c>
-      <c r="K22" s="14" t="n">
+      <c r="K22" s="66" t="n">
         <v>24.2</v>
       </c>
-      <c r="L22" s="14" t="n">
+      <c r="L22" s="66" t="n">
         <v>23.6</v>
       </c>
-      <c r="M22" s="14" t="n">
+      <c r="M22" s="66" t="n">
         <v>19.2</v>
       </c>
-      <c r="N22" s="14" t="n">
+      <c r="N22" s="66" t="n">
         <v>6.18</v>
       </c>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="29"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="114" t="n">
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="70"/>
+    </row>
+    <row r="23" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="115" t="n">
         <v>43047</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="73" t="s">
         <v>566</v>
       </c>
-      <c r="C23" s="39" t="n">
+      <c r="C23" s="81" t="n">
         <v>4.45</v>
       </c>
-      <c r="D23" s="39" t="n">
+      <c r="D23" s="81" t="n">
         <v>7.35</v>
       </c>
-      <c r="E23" s="39" t="n">
+      <c r="E23" s="81" t="n">
         <v>12.3</v>
       </c>
-      <c r="F23" s="39" t="n">
+      <c r="F23" s="81" t="n">
         <v>17.1</v>
       </c>
-      <c r="G23" s="39" t="n">
+      <c r="G23" s="81" t="n">
         <v>15</v>
       </c>
       <c r="H23" s="82" t="n">
         <v>13.3</v>
       </c>
-      <c r="I23" s="22" t="n">
+      <c r="I23" s="83" t="n">
         <v>12.5</v>
       </c>
-      <c r="J23" s="25" t="n">
+      <c r="J23" s="73" t="n">
         <v>11.3</v>
       </c>
-      <c r="K23" s="39" t="n">
+      <c r="K23" s="81" t="n">
         <v>8.25</v>
       </c>
-      <c r="L23" s="39" t="n">
+      <c r="L23" s="81" t="n">
         <v>4.18</v>
       </c>
-      <c r="M23" s="39" t="n">
+      <c r="M23" s="81" t="n">
         <v>3.49</v>
       </c>
-      <c r="N23" s="39" t="n">
+      <c r="N23" s="81" t="n">
         <v>3.37</v>
       </c>
-      <c r="O23" s="39"/>
+      <c r="O23" s="81"/>
       <c r="P23" s="82"/>
-      <c r="Q23" s="22"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="110" t="n">
+      <c r="Q23" s="83"/>
+    </row>
+    <row r="24" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="112" t="n">
         <v>42672</v>
       </c>
-      <c r="B24" s="99" t="s">
+      <c r="B24" s="102" t="s">
         <v>567</v>
       </c>
-      <c r="C24" s="20" t="n">
+      <c r="C24" s="94" t="n">
         <v>16.3</v>
       </c>
-      <c r="D24" s="20" t="n">
+      <c r="D24" s="94" t="n">
         <v>24.3</v>
       </c>
-      <c r="E24" s="20" t="n">
+      <c r="E24" s="94" t="n">
         <v>34.7</v>
       </c>
-      <c r="F24" s="20" t="n">
+      <c r="F24" s="94" t="n">
         <v>30.5</v>
       </c>
-      <c r="G24" s="20" t="n">
+      <c r="G24" s="94" t="n">
         <v>29.9</v>
       </c>
-      <c r="H24" s="20" t="n">
+      <c r="H24" s="94" t="n">
         <v>26</v>
       </c>
-      <c r="I24" s="20" t="n">
+      <c r="I24" s="94" t="n">
         <v>21.6</v>
       </c>
-      <c r="J24" s="20" t="n">
+      <c r="J24" s="94" t="n">
         <v>23.9</v>
       </c>
-      <c r="K24" s="20" t="n">
+      <c r="K24" s="94" t="n">
         <v>24.5</v>
       </c>
-      <c r="L24" s="20" t="n">
+      <c r="L24" s="94" t="n">
         <v>21.4</v>
       </c>
-      <c r="M24" s="91" t="n">
+      <c r="M24" s="93" t="n">
         <v>4.78</v>
       </c>
-      <c r="N24" s="91" t="n">
+      <c r="N24" s="93" t="n">
         <v>4.35</v>
       </c>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="29"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="114" t="n">
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="70"/>
+    </row>
+    <row r="25" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="115" t="n">
         <v>42994</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="73" t="s">
         <v>568</v>
       </c>
-      <c r="C25" s="39" t="n">
+      <c r="C25" s="81" t="n">
         <v>6.66</v>
       </c>
-      <c r="D25" s="39" t="n">
+      <c r="D25" s="81" t="n">
         <v>15.7</v>
       </c>
-      <c r="E25" s="39" t="n">
+      <c r="E25" s="81" t="n">
         <v>31</v>
       </c>
-      <c r="F25" s="39" t="n">
+      <c r="F25" s="81" t="n">
         <v>28.2</v>
       </c>
-      <c r="G25" s="39" t="n">
+      <c r="G25" s="81" t="n">
         <v>24.3</v>
       </c>
       <c r="H25" s="82" t="n">
         <v>21.2</v>
       </c>
-      <c r="I25" s="22" t="n">
+      <c r="I25" s="83" t="n">
         <v>18.8</v>
       </c>
-      <c r="J25" s="25" t="n">
+      <c r="J25" s="73" t="n">
         <v>17.1</v>
       </c>
-      <c r="K25" s="39" t="n">
+      <c r="K25" s="81" t="n">
         <v>14.9</v>
       </c>
-      <c r="L25" s="39" t="n">
+      <c r="L25" s="81" t="n">
         <v>13.1</v>
       </c>
-      <c r="M25" s="39" t="n">
+      <c r="M25" s="81" t="n">
         <v>12.6</v>
       </c>
-      <c r="N25" s="39" t="n">
+      <c r="N25" s="81" t="n">
         <v>6.06</v>
       </c>
-      <c r="O25" s="39" t="n">
+      <c r="O25" s="81" t="n">
         <v>5.59</v>
       </c>
       <c r="P25" s="82" t="n">
         <v>5.59</v>
       </c>
-      <c r="Q25" s="22" t="n">
+      <c r="Q25" s="83" t="n">
         <v>4.76</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="114" t="n">
+    <row r="26" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="115" t="n">
         <v>43034</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="73" t="s">
         <v>569</v>
       </c>
-      <c r="C26" s="39" t="n">
+      <c r="C26" s="81" t="n">
         <v>8.87</v>
       </c>
-      <c r="D26" s="39" t="n">
+      <c r="D26" s="81" t="n">
         <v>9.58</v>
       </c>
-      <c r="E26" s="39" t="n">
+      <c r="E26" s="81" t="n">
         <v>9.48</v>
       </c>
-      <c r="F26" s="39" t="n">
+      <c r="F26" s="81" t="n">
         <v>7.73</v>
       </c>
-      <c r="G26" s="39" t="n">
+      <c r="G26" s="81" t="n">
         <v>8.14</v>
       </c>
       <c r="H26" s="82" t="n">
         <v>9.04</v>
       </c>
-      <c r="I26" s="22" t="n">
+      <c r="I26" s="83" t="n">
         <v>8.23</v>
       </c>
-      <c r="J26" s="25" t="n">
+      <c r="J26" s="73" t="n">
         <v>7.32</v>
       </c>
-      <c r="K26" s="39" t="n">
+      <c r="K26" s="81" t="n">
         <v>6.8</v>
       </c>
-      <c r="L26" s="39" t="n">
+      <c r="L26" s="81" t="n">
         <v>7.78</v>
       </c>
-      <c r="M26" s="39" t="n">
+      <c r="M26" s="81" t="n">
         <v>6.42</v>
       </c>
-      <c r="N26" s="39" t="n">
+      <c r="N26" s="81" t="n">
         <v>6.83</v>
       </c>
-      <c r="O26" s="39" t="n">
+      <c r="O26" s="81" t="n">
         <v>6.38</v>
       </c>
       <c r="P26" s="82" t="n">
         <v>5.53</v>
       </c>
-      <c r="Q26" s="22" t="n">
+      <c r="Q26" s="83" t="n">
         <v>5.4</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18" t="n">
+    <row r="27" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="72" t="n">
         <v>42854</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="73" t="s">
         <v>570</v>
       </c>
-      <c r="C27" s="91" t="n">
+      <c r="C27" s="93" t="n">
         <v>3.95</v>
       </c>
-      <c r="D27" s="20" t="n">
+      <c r="D27" s="94" t="n">
         <v>10.7</v>
       </c>
-      <c r="E27" s="20" t="n">
+      <c r="E27" s="94" t="n">
         <v>17.7</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="94" t="n">
         <v>15.5</v>
       </c>
-      <c r="G27" s="20" t="n">
+      <c r="G27" s="94" t="n">
         <v>14.4</v>
       </c>
-      <c r="H27" s="20" t="n">
+      <c r="H27" s="94" t="n">
         <v>13.8</v>
       </c>
-      <c r="I27" s="20" t="n">
+      <c r="I27" s="94" t="n">
         <v>12.6</v>
       </c>
-      <c r="J27" s="91" t="n">
+      <c r="J27" s="93" t="n">
         <v>9.49</v>
       </c>
-      <c r="K27" s="91" t="n">
+      <c r="K27" s="93" t="n">
         <v>5.98</v>
       </c>
-      <c r="L27" s="91" t="n">
+      <c r="L27" s="93" t="n">
         <v>3.22</v>
       </c>
-      <c r="M27" s="91" t="n">
+      <c r="M27" s="93" t="n">
         <v>3.06</v>
       </c>
-      <c r="N27" s="91" t="n">
+      <c r="N27" s="93" t="n">
         <v>1.99</v>
       </c>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="29"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18" t="n">
+      <c r="O27" s="66"/>
+      <c r="P27" s="66"/>
+      <c r="Q27" s="70"/>
+    </row>
+    <row r="28" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="72" t="n">
         <v>42931</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="73" t="s">
         <v>570</v>
       </c>
-      <c r="C28" s="106" t="n">
+      <c r="C28" s="67" t="n">
         <v>7.58</v>
       </c>
-      <c r="D28" s="106" t="n">
+      <c r="D28" s="67" t="n">
         <v>8.37</v>
       </c>
-      <c r="E28" s="106" t="n">
+      <c r="E28" s="67" t="n">
         <v>8.27</v>
       </c>
-      <c r="F28" s="115" t="n">
+      <c r="F28" s="116" t="n">
         <v>8.4</v>
       </c>
-      <c r="G28" s="106" t="n">
+      <c r="G28" s="67" t="n">
         <v>8.47</v>
       </c>
-      <c r="H28" s="106" t="n">
+      <c r="H28" s="67" t="n">
         <v>8.52</v>
       </c>
-      <c r="I28" s="106" t="n">
+      <c r="I28" s="67" t="n">
         <v>8.14</v>
       </c>
-      <c r="J28" s="115" t="n">
+      <c r="J28" s="116" t="n">
         <v>7.4</v>
       </c>
-      <c r="K28" s="106" t="n">
+      <c r="K28" s="67" t="n">
         <v>7.04</v>
       </c>
-      <c r="L28" s="106" t="n">
+      <c r="L28" s="67" t="n">
         <v>6.81</v>
       </c>
-      <c r="M28" s="106" t="n">
+      <c r="M28" s="67" t="n">
         <v>6.77</v>
       </c>
-      <c r="N28" s="106" t="n">
+      <c r="N28" s="67" t="n">
         <v>5.31</v>
       </c>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="29"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="28" t="n">
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="70"/>
+    </row>
+    <row r="29" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="65" t="n">
         <v>42872</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="66" t="s">
         <v>571</v>
       </c>
-      <c r="C29" s="106" t="n">
+      <c r="C29" s="67" t="n">
         <v>6.08</v>
       </c>
-      <c r="D29" s="106" t="n">
+      <c r="D29" s="67" t="n">
         <v>7.74</v>
       </c>
-      <c r="E29" s="106" t="n">
+      <c r="E29" s="67" t="n">
         <v>11.7</v>
       </c>
-      <c r="F29" s="106" t="n">
+      <c r="F29" s="67" t="n">
         <v>10.1</v>
       </c>
-      <c r="G29" s="106" t="n">
+      <c r="G29" s="67" t="n">
         <v>9.96</v>
       </c>
-      <c r="H29" s="106" t="n">
+      <c r="H29" s="67" t="n">
         <v>10.7</v>
       </c>
-      <c r="I29" s="113" t="n">
+      <c r="I29" s="74" t="n">
         <v>11</v>
       </c>
-      <c r="J29" s="106" t="n">
+      <c r="J29" s="67" t="n">
         <v>9.67</v>
       </c>
-      <c r="K29" s="106" t="n">
+      <c r="K29" s="67" t="n">
         <v>12.3</v>
       </c>
-      <c r="L29" s="106" t="n">
+      <c r="L29" s="67" t="n">
         <v>6.02</v>
       </c>
-      <c r="M29" s="106" t="n">
+      <c r="M29" s="67" t="n">
         <v>5.18</v>
       </c>
-      <c r="N29" s="106" t="n">
+      <c r="N29" s="67" t="n">
         <v>4.78</v>
       </c>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="29"/>
+      <c r="O29" s="66"/>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="70"/>
     </row>
     <row r="30" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="76" t="n">
@@ -26827,45 +26911,45 @@
       <c r="B30" s="73" t="s">
         <v>572</v>
       </c>
-      <c r="C30" s="116" t="n">
+      <c r="C30" s="81" t="n">
         <v>1.73</v>
       </c>
-      <c r="D30" s="116" t="n">
+      <c r="D30" s="81" t="n">
         <v>23.1</v>
       </c>
-      <c r="E30" s="116" t="n">
+      <c r="E30" s="81" t="n">
         <v>4.67</v>
       </c>
-      <c r="F30" s="116" t="n">
+      <c r="F30" s="81" t="n">
         <v>4.19</v>
       </c>
-      <c r="G30" s="116" t="n">
+      <c r="G30" s="81" t="n">
         <v>4.88</v>
       </c>
-      <c r="H30" s="117" t="n">
+      <c r="H30" s="82" t="n">
         <v>3.79</v>
       </c>
-      <c r="I30" s="118" t="n">
+      <c r="I30" s="83" t="n">
         <v>2.18</v>
       </c>
       <c r="J30" s="73" t="n">
         <v>2.12</v>
       </c>
-      <c r="K30" s="116" t="n">
+      <c r="K30" s="81" t="n">
         <v>1.73</v>
       </c>
-      <c r="L30" s="116" t="n">
+      <c r="L30" s="81" t="n">
         <v>1.9</v>
       </c>
-      <c r="M30" s="116" t="n">
+      <c r="M30" s="81" t="n">
         <v>2.33</v>
       </c>
-      <c r="N30" s="116" t="n">
+      <c r="N30" s="81" t="n">
         <v>1.36</v>
       </c>
-      <c r="O30" s="116"/>
-      <c r="P30" s="117"/>
-      <c r="Q30" s="118"/>
+      <c r="O30" s="81"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="83"/>
     </row>
     <row r="31" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="72" t="n">
@@ -26921,40 +27005,40 @@
       <c r="B32" s="73" t="s">
         <v>574</v>
       </c>
-      <c r="C32" s="119" t="n">
+      <c r="C32" s="93" t="n">
         <v>5.54</v>
       </c>
-      <c r="D32" s="119" t="n">
+      <c r="D32" s="93" t="n">
         <v>3.96</v>
       </c>
-      <c r="E32" s="119" t="n">
+      <c r="E32" s="93" t="n">
         <v>3.06</v>
       </c>
-      <c r="F32" s="120" t="n">
+      <c r="F32" s="94" t="n">
         <v>12.5</v>
       </c>
-      <c r="G32" s="120" t="n">
+      <c r="G32" s="94" t="n">
         <v>26.9</v>
       </c>
-      <c r="H32" s="120" t="n">
+      <c r="H32" s="94" t="n">
         <v>14.2</v>
       </c>
-      <c r="I32" s="120" t="n">
+      <c r="I32" s="94" t="n">
         <v>13.2</v>
       </c>
-      <c r="J32" s="120" t="n">
+      <c r="J32" s="94" t="n">
         <v>30.9</v>
       </c>
-      <c r="K32" s="120" t="n">
+      <c r="K32" s="94" t="n">
         <v>20.6</v>
       </c>
-      <c r="L32" s="119" t="n">
+      <c r="L32" s="93" t="n">
         <v>5.13</v>
       </c>
-      <c r="M32" s="119" t="n">
+      <c r="M32" s="93" t="n">
         <v>9.49</v>
       </c>
-      <c r="N32" s="119" t="n">
+      <c r="N32" s="93" t="n">
         <v>2.79</v>
       </c>
       <c r="O32" s="75"/>
@@ -26968,40 +27052,40 @@
       <c r="B33" s="73" t="s">
         <v>574</v>
       </c>
-      <c r="C33" s="120" t="n">
+      <c r="C33" s="94" t="n">
         <v>13.1</v>
       </c>
-      <c r="D33" s="121" t="n">
+      <c r="D33" s="117" t="n">
         <v>3</v>
       </c>
-      <c r="E33" s="119" t="n">
+      <c r="E33" s="93" t="n">
         <v>3.05</v>
       </c>
-      <c r="F33" s="119" t="n">
+      <c r="F33" s="93" t="n">
         <v>3.84</v>
       </c>
-      <c r="G33" s="119" t="n">
+      <c r="G33" s="93" t="n">
         <v>6.53</v>
       </c>
-      <c r="H33" s="119" t="n">
+      <c r="H33" s="93" t="n">
         <v>8.34</v>
       </c>
-      <c r="I33" s="120" t="n">
+      <c r="I33" s="94" t="n">
         <v>11.6</v>
       </c>
-      <c r="J33" s="119" t="n">
+      <c r="J33" s="93" t="n">
         <v>9.71</v>
       </c>
-      <c r="K33" s="119" t="n">
+      <c r="K33" s="93" t="n">
         <v>9.46</v>
       </c>
-      <c r="L33" s="120" t="n">
+      <c r="L33" s="94" t="n">
         <v>14.4</v>
       </c>
-      <c r="M33" s="120" t="n">
+      <c r="M33" s="94" t="n">
         <v>8.2</v>
       </c>
-      <c r="N33" s="119" t="n">
+      <c r="N33" s="93" t="n">
         <v>3.1</v>
       </c>
       <c r="O33" s="70" t="n">
@@ -27021,16 +27105,16 @@
       <c r="B34" s="66" t="s">
         <v>575</v>
       </c>
-      <c r="C34" s="122" t="n">
+      <c r="C34" s="116" t="n">
         <v>5.12</v>
       </c>
-      <c r="D34" s="119" t="n">
+      <c r="D34" s="93" t="n">
         <v>6.39</v>
       </c>
-      <c r="E34" s="119" t="n">
+      <c r="E34" s="93" t="n">
         <v>6.69</v>
       </c>
-      <c r="F34" s="119" t="n">
+      <c r="F34" s="93" t="n">
         <v>7.95</v>
       </c>
       <c r="G34" s="70" t="n">
@@ -27065,22 +27149,22 @@
       <c r="A35" s="55" t="s">
         <v>529</v>
       </c>
-      <c r="B35" s="123"/>
-      <c r="C35" s="123"/>
-      <c r="D35" s="123"/>
-      <c r="E35" s="123"/>
-      <c r="F35" s="123"/>
-      <c r="G35" s="123"/>
-      <c r="H35" s="123"/>
-      <c r="I35" s="123"/>
-      <c r="J35" s="123"/>
-      <c r="K35" s="123"/>
-      <c r="L35" s="123"/>
-      <c r="M35" s="123"/>
-      <c r="N35" s="123"/>
-      <c r="O35" s="123"/>
-      <c r="P35" s="123"/>
-      <c r="Q35" s="123"/>
+      <c r="B35" s="118"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="118"/>
+      <c r="K35" s="118"/>
+      <c r="L35" s="118"/>
+      <c r="M35" s="118"/>
+      <c r="N35" s="118"/>
+      <c r="O35" s="118"/>
+      <c r="P35" s="118"/>
+      <c r="Q35" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -27110,7 +27194,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>#ref!="TBS"</formula>
+      <formula>#REF!="TBS"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>